<commit_message>
try to sent att log file
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D20B18-CEA5-4C43-81B8-5E4963D632B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2484C3B-04CF-4D19-8C9F-ECF63DCD1ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,12 +216,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -251,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -260,6 +266,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,8 +611,8 @@
   </sheetPr>
   <dimension ref="A7:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,21 +663,21 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
websocket disable when lost wifi
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2484C3B-04CF-4D19-8C9F-ECF63DCD1ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F31151-616A-4305-93B5-48F65CBC2047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>ping</t>
   </si>
@@ -50,9 +50,6 @@
     <t>attendance log</t>
   </si>
   <si>
-    <t>device time+log time + person id + Device id</t>
-  </si>
-  <si>
     <t>cmd</t>
   </si>
   <si>
@@ -86,33 +83,18 @@
     <t>enrol timeout</t>
   </si>
   <si>
-    <t>NETO+divece id</t>
-  </si>
-  <si>
-    <t>NDP+id+device id</t>
-  </si>
-  <si>
     <t>person delete done</t>
   </si>
   <si>
-    <t>ADI+person id+ device id</t>
-  </si>
-  <si>
     <t>invalide id</t>
   </si>
   <si>
-    <t>NDII+person id+ device id</t>
-  </si>
-  <si>
     <t>Subscribed Topic</t>
   </si>
   <si>
     <t>person delete request</t>
   </si>
   <si>
-    <t>cmddl+person id+cmdend</t>
-  </si>
-  <si>
     <t xml:space="preserve">update time request </t>
   </si>
   <si>
@@ -123,9 +105,6 @@
   </si>
   <si>
     <t>dump sent</t>
-  </si>
-  <si>
-    <t>device status data+ device id</t>
   </si>
   <si>
     <t>from server</t>
@@ -156,9 +135,6 @@
     </r>
   </si>
   <si>
-    <t>AED+person name+ Id +crc value + device id</t>
-  </si>
-  <si>
     <t>from device NDII= Nack for delete invalide id</t>
   </si>
   <si>
@@ -187,6 +163,33 @@
   </si>
   <si>
     <t>yyyy-mm-dd-hh-mm-ss-24H/12H</t>
+  </si>
+  <si>
+    <t>device time+log time + person id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AED+person name+ Id +crc value </t>
+  </si>
+  <si>
+    <t>NDP+id</t>
+  </si>
+  <si>
+    <t>NETO</t>
+  </si>
+  <si>
+    <t>device status data</t>
+  </si>
+  <si>
+    <t>cmddl+person id</t>
+  </si>
+  <si>
+    <t>ADI+person id</t>
+  </si>
+  <si>
+    <t>NDII+person id</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <dimension ref="A7:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,21 +623,21 @@
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" customWidth="1"/>
-    <col min="4" max="4" width="83.42578125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -644,13 +647,13 @@
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -668,13 +671,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -692,13 +698,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -706,37 +712,37 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -747,64 +753,64 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -815,16 +821,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now trying on event logic
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C976FCBA-3CCF-4938-8CD9-A2A98F4EACF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735BE202-9C43-4107-8BF8-19B319BC9C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
   <dimension ref="A7:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -712,7 +712,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
enrollment on going but device is restarting when sent enrol cmd
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735BE202-9C43-4107-8BF8-19B319BC9C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4B8293-9DB6-45ED-B569-9E6C24E4FE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$7:$D$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$7:$D$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>ping</t>
   </si>
@@ -159,24 +159,12 @@
     <t xml:space="preserve">AED+person name+ Id +crc value </t>
   </si>
   <si>
-    <t>NDP+id</t>
-  </si>
-  <si>
     <t>NETO</t>
   </si>
   <si>
     <t>device status data</t>
   </si>
   <si>
-    <t>cmddl+person id</t>
-  </si>
-  <si>
-    <t>ADI+person id</t>
-  </si>
-  <si>
-    <t>NDII+person id</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -193,6 +181,36 @@
   </si>
   <si>
     <t>Time ping always 24H</t>
+  </si>
+  <si>
+    <t>id crc error</t>
+  </si>
+  <si>
+    <t>NIDE</t>
+  </si>
+  <si>
+    <t>NDII</t>
+  </si>
+  <si>
+    <t>ADI</t>
+  </si>
+  <si>
+    <t>cmddl+person id cndend</t>
+  </si>
+  <si>
+    <t>NIDE= nack for id data error</t>
+  </si>
+  <si>
+    <t>name crc error</t>
+  </si>
+  <si>
+    <t>NNDE</t>
+  </si>
+  <si>
+    <t>NDP</t>
+  </si>
+  <si>
+    <t>NNDE = Nack for name data error</t>
   </si>
 </sst>
 </file>
@@ -263,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -278,6 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,10 +634,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A7:L24"/>
+  <dimension ref="A7:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,17 +665,17 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>44</v>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -677,13 +696,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -730,7 +749,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>29</v>
@@ -739,106 +758,136 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enrolment done via rtoss
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4B8293-9DB6-45ED-B569-9E6C24E4FE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53770909-AD64-4C4D-B736-54A64149DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -217,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,8 +239,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +256,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -296,7 +308,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +652,7 @@
   <dimension ref="A7:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,42 +731,42 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -768,14 +783,14 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -860,14 +875,14 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
face frame Aline add but when aline face print then time out not work
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53770909-AD64-4C4D-B736-54A64149DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCEB583-1D3E-4920-A08C-BF64A955516A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A7:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cpu bg flag clear and can sent to ack
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCEB583-1D3E-4920-A08C-BF64A955516A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FD108F-EB08-4BE9-8370-89EDE47F3C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A7:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pic save in fatfs and re display image done by using drawimage
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FD108F-EB08-4BE9-8370-89EDE47F3C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51412F28-75E3-4C35-8168-65A8443860BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$7:$D$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -293,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -305,13 +306,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,10 +651,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A7:L27"/>
+  <dimension ref="A7:AHY27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +665,7 @@
     <col min="4" max="4" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:909" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -679,7 +681,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:909" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -695,7 +697,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:909" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -703,7 +705,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:909" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
@@ -716,13 +718,915 @@
       <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+      <c r="AX10" s="9"/>
+      <c r="AY10" s="9"/>
+      <c r="AZ10" s="9"/>
+      <c r="BA10" s="9"/>
+      <c r="BB10" s="9"/>
+      <c r="BC10" s="9"/>
+      <c r="BD10" s="9"/>
+      <c r="BE10" s="9"/>
+      <c r="BF10" s="9"/>
+      <c r="BG10" s="9"/>
+      <c r="BH10" s="9"/>
+      <c r="BI10" s="9"/>
+      <c r="BJ10" s="9"/>
+      <c r="BK10" s="9"/>
+      <c r="BL10" s="9"/>
+      <c r="BM10" s="9"/>
+      <c r="BN10" s="9"/>
+      <c r="BO10" s="9"/>
+      <c r="BP10" s="9"/>
+      <c r="BQ10" s="9"/>
+      <c r="BR10" s="9"/>
+      <c r="BS10" s="9"/>
+      <c r="BT10" s="9"/>
+      <c r="BU10" s="9"/>
+      <c r="BV10" s="9"/>
+      <c r="BW10" s="9"/>
+      <c r="BX10" s="9"/>
+      <c r="BY10" s="9"/>
+      <c r="BZ10" s="9"/>
+      <c r="CA10" s="9"/>
+      <c r="CB10" s="9"/>
+      <c r="CC10" s="9"/>
+      <c r="CD10" s="9"/>
+      <c r="CE10" s="9"/>
+      <c r="CF10" s="9"/>
+      <c r="CG10" s="9"/>
+      <c r="CH10" s="9"/>
+      <c r="CI10" s="9"/>
+      <c r="CJ10" s="9"/>
+      <c r="CK10" s="9"/>
+      <c r="CL10" s="9"/>
+      <c r="CM10" s="9"/>
+      <c r="CN10" s="9"/>
+      <c r="CO10" s="9"/>
+      <c r="CP10" s="9"/>
+      <c r="CQ10" s="9"/>
+      <c r="CR10" s="9"/>
+      <c r="CS10" s="9"/>
+      <c r="CT10" s="9"/>
+      <c r="CU10" s="9"/>
+      <c r="CV10" s="9"/>
+      <c r="CW10" s="9"/>
+      <c r="CX10" s="9"/>
+      <c r="CY10" s="9"/>
+      <c r="CZ10" s="9"/>
+      <c r="DA10" s="9"/>
+      <c r="DB10" s="9"/>
+      <c r="DC10" s="9"/>
+      <c r="DD10" s="9"/>
+      <c r="DE10" s="9"/>
+      <c r="DF10" s="9"/>
+      <c r="DG10" s="9"/>
+      <c r="DH10" s="9"/>
+      <c r="DI10" s="9"/>
+      <c r="DJ10" s="9"/>
+      <c r="DK10" s="9"/>
+      <c r="DL10" s="9"/>
+      <c r="DM10" s="9"/>
+      <c r="DN10" s="9"/>
+      <c r="DO10" s="9"/>
+      <c r="DP10" s="9"/>
+      <c r="DQ10" s="9"/>
+      <c r="DR10" s="9"/>
+      <c r="DS10" s="9"/>
+      <c r="DT10" s="9"/>
+      <c r="DU10" s="9"/>
+      <c r="DV10" s="9"/>
+      <c r="DW10" s="9"/>
+      <c r="DX10" s="9"/>
+      <c r="DY10" s="9"/>
+      <c r="DZ10" s="9"/>
+      <c r="EA10" s="9"/>
+      <c r="EB10" s="9"/>
+      <c r="EC10" s="9"/>
+      <c r="ED10" s="9"/>
+      <c r="EE10" s="9"/>
+      <c r="EF10" s="9"/>
+      <c r="EG10" s="9"/>
+      <c r="EH10" s="9"/>
+      <c r="EI10" s="9"/>
+      <c r="EJ10" s="9"/>
+      <c r="EK10" s="9"/>
+      <c r="EL10" s="9"/>
+      <c r="EM10" s="9"/>
+      <c r="EN10" s="9"/>
+      <c r="EO10" s="9"/>
+      <c r="EP10" s="9"/>
+      <c r="EQ10" s="9"/>
+      <c r="ER10" s="9"/>
+      <c r="ES10" s="9"/>
+      <c r="ET10" s="9"/>
+      <c r="EU10" s="9"/>
+      <c r="EV10" s="9"/>
+      <c r="EW10" s="9"/>
+      <c r="EX10" s="9"/>
+      <c r="EY10" s="9"/>
+      <c r="EZ10" s="9"/>
+      <c r="FA10" s="9"/>
+      <c r="FB10" s="9"/>
+      <c r="FC10" s="9"/>
+      <c r="FD10" s="9"/>
+      <c r="FE10" s="9"/>
+      <c r="FF10" s="9"/>
+      <c r="FG10" s="9"/>
+      <c r="FH10" s="9"/>
+      <c r="FI10" s="9"/>
+      <c r="FJ10" s="9"/>
+      <c r="FK10" s="9"/>
+      <c r="FL10" s="9"/>
+      <c r="FM10" s="9"/>
+      <c r="FN10" s="9"/>
+      <c r="FO10" s="9"/>
+      <c r="FP10" s="9"/>
+      <c r="FQ10" s="9"/>
+      <c r="FR10" s="9"/>
+      <c r="FS10" s="9"/>
+      <c r="FT10" s="9"/>
+      <c r="FU10" s="9"/>
+      <c r="FV10" s="9"/>
+      <c r="FW10" s="9"/>
+      <c r="FX10" s="9"/>
+      <c r="FY10" s="9"/>
+      <c r="FZ10" s="9"/>
+      <c r="GA10" s="9"/>
+      <c r="GB10" s="9"/>
+      <c r="GC10" s="9"/>
+      <c r="GD10" s="9"/>
+      <c r="GE10" s="9"/>
+      <c r="GF10" s="9"/>
+      <c r="GG10" s="9"/>
+      <c r="GH10" s="9"/>
+      <c r="GI10" s="9"/>
+      <c r="GJ10" s="9"/>
+      <c r="GK10" s="9"/>
+      <c r="GL10" s="9"/>
+      <c r="GM10" s="9"/>
+      <c r="GN10" s="9"/>
+      <c r="GO10" s="9"/>
+      <c r="GP10" s="9"/>
+      <c r="GQ10" s="9"/>
+      <c r="GR10" s="9"/>
+      <c r="GS10" s="9"/>
+      <c r="GT10" s="9"/>
+      <c r="GU10" s="9"/>
+      <c r="GV10" s="9"/>
+      <c r="GW10" s="9"/>
+      <c r="GX10" s="9"/>
+      <c r="GY10" s="9"/>
+      <c r="GZ10" s="9"/>
+      <c r="HA10" s="9"/>
+      <c r="HB10" s="9"/>
+      <c r="HC10" s="9"/>
+      <c r="HD10" s="9"/>
+      <c r="HE10" s="9"/>
+      <c r="HF10" s="9"/>
+      <c r="HG10" s="9"/>
+      <c r="HH10" s="9"/>
+      <c r="HI10" s="9"/>
+      <c r="HJ10" s="9"/>
+      <c r="HK10" s="9"/>
+      <c r="HL10" s="9"/>
+      <c r="HM10" s="9"/>
+      <c r="HN10" s="9"/>
+      <c r="HO10" s="9"/>
+      <c r="HP10" s="9"/>
+      <c r="HQ10" s="9"/>
+      <c r="HR10" s="9"/>
+      <c r="HS10" s="9"/>
+      <c r="HT10" s="9"/>
+      <c r="HU10" s="9"/>
+      <c r="HV10" s="9"/>
+      <c r="HW10" s="9"/>
+      <c r="HX10" s="9"/>
+      <c r="HY10" s="9"/>
+      <c r="HZ10" s="9"/>
+      <c r="IA10" s="9"/>
+      <c r="IB10" s="9"/>
+      <c r="IC10" s="9"/>
+      <c r="ID10" s="9"/>
+      <c r="IE10" s="9"/>
+      <c r="IF10" s="9"/>
+      <c r="IG10" s="9"/>
+      <c r="IH10" s="9"/>
+      <c r="II10" s="9"/>
+      <c r="IJ10" s="9"/>
+      <c r="IK10" s="9"/>
+      <c r="IL10" s="9"/>
+      <c r="IM10" s="9"/>
+      <c r="IN10" s="9"/>
+      <c r="IO10" s="9"/>
+      <c r="IP10" s="9"/>
+      <c r="IQ10" s="9"/>
+      <c r="IR10" s="9"/>
+      <c r="IS10" s="9"/>
+      <c r="IT10" s="9"/>
+      <c r="IU10" s="9"/>
+      <c r="IV10" s="9"/>
+      <c r="IW10" s="9"/>
+      <c r="IX10" s="9"/>
+      <c r="IY10" s="9"/>
+      <c r="IZ10" s="9"/>
+      <c r="JA10" s="9"/>
+      <c r="JB10" s="9"/>
+      <c r="JC10" s="9"/>
+      <c r="JD10" s="9"/>
+      <c r="JE10" s="9"/>
+      <c r="JF10" s="9"/>
+      <c r="JG10" s="9"/>
+      <c r="JH10" s="9"/>
+      <c r="JI10" s="9"/>
+      <c r="JJ10" s="9"/>
+      <c r="JK10" s="9"/>
+      <c r="JL10" s="9"/>
+      <c r="JM10" s="9"/>
+      <c r="JN10" s="9"/>
+      <c r="JO10" s="9"/>
+      <c r="JP10" s="9"/>
+      <c r="JQ10" s="9"/>
+      <c r="JR10" s="9"/>
+      <c r="JS10" s="9"/>
+      <c r="JT10" s="9"/>
+      <c r="JU10" s="9"/>
+      <c r="JV10" s="9"/>
+      <c r="JW10" s="9"/>
+      <c r="JX10" s="9"/>
+      <c r="JY10" s="9"/>
+      <c r="JZ10" s="9"/>
+      <c r="KA10" s="9"/>
+      <c r="KB10" s="9"/>
+      <c r="KC10" s="9"/>
+      <c r="KD10" s="9"/>
+      <c r="KE10" s="9"/>
+      <c r="KF10" s="9"/>
+      <c r="KG10" s="9"/>
+      <c r="KH10" s="9"/>
+      <c r="KI10" s="9"/>
+      <c r="KJ10" s="9"/>
+      <c r="KK10" s="9"/>
+      <c r="KL10" s="9"/>
+      <c r="KM10" s="9"/>
+      <c r="KN10" s="9"/>
+      <c r="KO10" s="9"/>
+      <c r="KP10" s="9"/>
+      <c r="KQ10" s="9"/>
+      <c r="KR10" s="9"/>
+      <c r="KS10" s="9"/>
+      <c r="KT10" s="9"/>
+      <c r="KU10" s="9"/>
+      <c r="KV10" s="9"/>
+      <c r="KW10" s="9"/>
+      <c r="KX10" s="9"/>
+      <c r="KY10" s="9"/>
+      <c r="KZ10" s="9"/>
+      <c r="LA10" s="9"/>
+      <c r="LB10" s="9"/>
+      <c r="LC10" s="9"/>
+      <c r="LD10" s="9"/>
+      <c r="LE10" s="9"/>
+      <c r="LF10" s="9"/>
+      <c r="LG10" s="9"/>
+      <c r="LH10" s="9"/>
+      <c r="LI10" s="9"/>
+      <c r="LJ10" s="9"/>
+      <c r="LK10" s="9"/>
+      <c r="LL10" s="9"/>
+      <c r="LM10" s="9"/>
+      <c r="LN10" s="9"/>
+      <c r="LO10" s="9"/>
+      <c r="LP10" s="9"/>
+      <c r="LQ10" s="9"/>
+      <c r="LR10" s="9"/>
+      <c r="LS10" s="9"/>
+      <c r="LT10" s="9"/>
+      <c r="LU10" s="9"/>
+      <c r="LV10" s="9"/>
+      <c r="LW10" s="9"/>
+      <c r="LX10" s="9"/>
+      <c r="LY10" s="9"/>
+      <c r="LZ10" s="9"/>
+      <c r="MA10" s="9"/>
+      <c r="MB10" s="9"/>
+      <c r="MC10" s="9"/>
+      <c r="MD10" s="9"/>
+      <c r="ME10" s="9"/>
+      <c r="MF10" s="9"/>
+      <c r="MG10" s="9"/>
+      <c r="MH10" s="9"/>
+      <c r="MI10" s="9"/>
+      <c r="MJ10" s="9"/>
+      <c r="MK10" s="9"/>
+      <c r="ML10" s="9"/>
+      <c r="MM10" s="9"/>
+      <c r="MN10" s="9"/>
+      <c r="MO10" s="9"/>
+      <c r="MP10" s="9"/>
+      <c r="MQ10" s="9"/>
+      <c r="MR10" s="9"/>
+      <c r="MS10" s="9"/>
+      <c r="MT10" s="9"/>
+      <c r="MU10" s="9"/>
+      <c r="MV10" s="9"/>
+      <c r="MW10" s="9"/>
+      <c r="MX10" s="9"/>
+      <c r="MY10" s="9"/>
+      <c r="MZ10" s="9"/>
+      <c r="NA10" s="9"/>
+      <c r="NB10" s="9"/>
+      <c r="NC10" s="9"/>
+      <c r="ND10" s="9"/>
+      <c r="NE10" s="9"/>
+      <c r="NF10" s="9"/>
+      <c r="NG10" s="9"/>
+      <c r="NH10" s="9"/>
+      <c r="NI10" s="9"/>
+      <c r="NJ10" s="9"/>
+      <c r="NK10" s="9"/>
+      <c r="NL10" s="9"/>
+      <c r="NM10" s="9"/>
+      <c r="NN10" s="9"/>
+      <c r="NO10" s="9"/>
+      <c r="NP10" s="9"/>
+      <c r="NQ10" s="9"/>
+      <c r="NR10" s="9"/>
+      <c r="NS10" s="9"/>
+      <c r="NT10" s="9"/>
+      <c r="NU10" s="9"/>
+      <c r="NV10" s="9"/>
+      <c r="NW10" s="9"/>
+      <c r="NX10" s="9"/>
+      <c r="NY10" s="9"/>
+      <c r="NZ10" s="9"/>
+      <c r="OA10" s="9"/>
+      <c r="OB10" s="9"/>
+      <c r="OC10" s="9"/>
+      <c r="OD10" s="9"/>
+      <c r="OE10" s="9"/>
+      <c r="OF10" s="9"/>
+      <c r="OG10" s="9"/>
+      <c r="OH10" s="9"/>
+      <c r="OI10" s="9"/>
+      <c r="OJ10" s="9"/>
+      <c r="OK10" s="9"/>
+      <c r="OL10" s="9"/>
+      <c r="OM10" s="9"/>
+      <c r="ON10" s="9"/>
+      <c r="OO10" s="9"/>
+      <c r="OP10" s="9"/>
+      <c r="OQ10" s="9"/>
+      <c r="OR10" s="9"/>
+      <c r="OS10" s="9"/>
+      <c r="OT10" s="9"/>
+      <c r="OU10" s="9"/>
+      <c r="OV10" s="9"/>
+      <c r="OW10" s="9"/>
+      <c r="OX10" s="9"/>
+      <c r="OY10" s="9"/>
+      <c r="OZ10" s="9"/>
+      <c r="PA10" s="9"/>
+      <c r="PB10" s="9"/>
+      <c r="PC10" s="9"/>
+      <c r="PD10" s="9"/>
+      <c r="PE10" s="9"/>
+      <c r="PF10" s="9"/>
+      <c r="PG10" s="9"/>
+      <c r="PH10" s="9"/>
+      <c r="PI10" s="9"/>
+      <c r="PJ10" s="9"/>
+      <c r="PK10" s="9"/>
+      <c r="PL10" s="9"/>
+      <c r="PM10" s="9"/>
+      <c r="PN10" s="9"/>
+      <c r="PO10" s="9"/>
+      <c r="PP10" s="9"/>
+      <c r="PQ10" s="9"/>
+      <c r="PR10" s="9"/>
+      <c r="PS10" s="9"/>
+      <c r="PT10" s="9"/>
+      <c r="PU10" s="9"/>
+      <c r="PV10" s="9"/>
+      <c r="PW10" s="9"/>
+      <c r="PX10" s="9"/>
+      <c r="PY10" s="9"/>
+      <c r="PZ10" s="9"/>
+      <c r="QA10" s="9"/>
+      <c r="QB10" s="9"/>
+      <c r="QC10" s="9"/>
+      <c r="QD10" s="9"/>
+      <c r="QE10" s="9"/>
+      <c r="QF10" s="9"/>
+      <c r="QG10" s="9"/>
+      <c r="QH10" s="9"/>
+      <c r="QI10" s="9"/>
+      <c r="QJ10" s="9"/>
+      <c r="QK10" s="9"/>
+      <c r="QL10" s="9"/>
+      <c r="QM10" s="9"/>
+      <c r="QN10" s="9"/>
+      <c r="QO10" s="9"/>
+      <c r="QP10" s="9"/>
+      <c r="QQ10" s="9"/>
+      <c r="QR10" s="9"/>
+      <c r="QS10" s="9"/>
+      <c r="QT10" s="9"/>
+      <c r="QU10" s="9"/>
+      <c r="QV10" s="9"/>
+      <c r="QW10" s="9"/>
+      <c r="QX10" s="9"/>
+      <c r="QY10" s="9"/>
+      <c r="QZ10" s="9"/>
+      <c r="RA10" s="9"/>
+      <c r="RB10" s="9"/>
+      <c r="RC10" s="9"/>
+      <c r="RD10" s="9"/>
+      <c r="RE10" s="9"/>
+      <c r="RF10" s="9"/>
+      <c r="RG10" s="9"/>
+      <c r="RH10" s="9"/>
+      <c r="RI10" s="9"/>
+      <c r="RJ10" s="9"/>
+      <c r="RK10" s="9"/>
+      <c r="RL10" s="9"/>
+      <c r="RM10" s="9"/>
+      <c r="RN10" s="9"/>
+      <c r="RO10" s="9"/>
+      <c r="RP10" s="9"/>
+      <c r="RQ10" s="9"/>
+      <c r="RR10" s="9"/>
+      <c r="RS10" s="9"/>
+      <c r="RT10" s="9"/>
+      <c r="RU10" s="9"/>
+      <c r="RV10" s="9"/>
+      <c r="RW10" s="9"/>
+      <c r="RX10" s="9"/>
+      <c r="RY10" s="9"/>
+      <c r="RZ10" s="9"/>
+      <c r="SA10" s="9"/>
+      <c r="SB10" s="9"/>
+      <c r="SC10" s="9"/>
+      <c r="SD10" s="9"/>
+      <c r="SE10" s="9"/>
+      <c r="SF10" s="9"/>
+      <c r="SG10" s="9"/>
+      <c r="SH10" s="9"/>
+      <c r="SI10" s="9"/>
+      <c r="SJ10" s="9"/>
+      <c r="SK10" s="9"/>
+      <c r="SL10" s="9"/>
+      <c r="SM10" s="9"/>
+      <c r="SN10" s="9"/>
+      <c r="SO10" s="9"/>
+      <c r="SP10" s="9"/>
+      <c r="SQ10" s="9"/>
+      <c r="SR10" s="9"/>
+      <c r="SS10" s="9"/>
+      <c r="ST10" s="9"/>
+      <c r="SU10" s="9"/>
+      <c r="SV10" s="9"/>
+      <c r="SW10" s="9"/>
+      <c r="SX10" s="9"/>
+      <c r="SY10" s="9"/>
+      <c r="SZ10" s="9"/>
+      <c r="TA10" s="9"/>
+      <c r="TB10" s="9"/>
+      <c r="TC10" s="9"/>
+      <c r="TD10" s="9"/>
+      <c r="TE10" s="9"/>
+      <c r="TF10" s="9"/>
+      <c r="TG10" s="9"/>
+      <c r="TH10" s="9"/>
+      <c r="TI10" s="9"/>
+      <c r="TJ10" s="9"/>
+      <c r="TK10" s="9"/>
+      <c r="TL10" s="9"/>
+      <c r="TM10" s="9"/>
+      <c r="TN10" s="9"/>
+      <c r="TO10" s="9"/>
+      <c r="TP10" s="9"/>
+      <c r="TQ10" s="9"/>
+      <c r="TR10" s="9"/>
+      <c r="TS10" s="9"/>
+      <c r="TT10" s="9"/>
+      <c r="TU10" s="9"/>
+      <c r="TV10" s="9"/>
+      <c r="TW10" s="9"/>
+      <c r="TX10" s="9"/>
+      <c r="TY10" s="9"/>
+      <c r="TZ10" s="9"/>
+      <c r="UA10" s="9"/>
+      <c r="UB10" s="9"/>
+      <c r="UC10" s="9"/>
+      <c r="UD10" s="9"/>
+      <c r="UE10" s="9"/>
+      <c r="UF10" s="9"/>
+      <c r="UG10" s="9"/>
+      <c r="UH10" s="9"/>
+      <c r="UI10" s="9"/>
+      <c r="UJ10" s="9"/>
+      <c r="UK10" s="9"/>
+      <c r="UL10" s="9"/>
+      <c r="UM10" s="9"/>
+      <c r="UN10" s="9"/>
+      <c r="UO10" s="9"/>
+      <c r="UP10" s="9"/>
+      <c r="UQ10" s="9"/>
+      <c r="UR10" s="9"/>
+      <c r="US10" s="9"/>
+      <c r="UT10" s="9"/>
+      <c r="UU10" s="9"/>
+      <c r="UV10" s="9"/>
+      <c r="UW10" s="9"/>
+      <c r="UX10" s="9"/>
+      <c r="UY10" s="9"/>
+      <c r="UZ10" s="9"/>
+      <c r="VA10" s="9"/>
+      <c r="VB10" s="9"/>
+      <c r="VC10" s="9"/>
+      <c r="VD10" s="9"/>
+      <c r="VE10" s="9"/>
+      <c r="VF10" s="9"/>
+      <c r="VG10" s="9"/>
+      <c r="VH10" s="9"/>
+      <c r="VI10" s="9"/>
+      <c r="VJ10" s="9"/>
+      <c r="VK10" s="9"/>
+      <c r="VL10" s="9"/>
+      <c r="VM10" s="9"/>
+      <c r="VN10" s="9"/>
+      <c r="VO10" s="9"/>
+      <c r="VP10" s="9"/>
+      <c r="VQ10" s="9"/>
+      <c r="VR10" s="9"/>
+      <c r="VS10" s="9"/>
+      <c r="VT10" s="9"/>
+      <c r="VU10" s="9"/>
+      <c r="VV10" s="9"/>
+      <c r="VW10" s="9"/>
+      <c r="VX10" s="9"/>
+      <c r="VY10" s="9"/>
+      <c r="VZ10" s="9"/>
+      <c r="WA10" s="9"/>
+      <c r="WB10" s="9"/>
+      <c r="WC10" s="9"/>
+      <c r="WD10" s="9"/>
+      <c r="WE10" s="9"/>
+      <c r="WF10" s="9"/>
+      <c r="WG10" s="9"/>
+      <c r="WH10" s="9"/>
+      <c r="WI10" s="9"/>
+      <c r="WJ10" s="9"/>
+      <c r="WK10" s="9"/>
+      <c r="WL10" s="9"/>
+      <c r="WM10" s="9"/>
+      <c r="WN10" s="9"/>
+      <c r="WO10" s="9"/>
+      <c r="WP10" s="9"/>
+      <c r="WQ10" s="9"/>
+      <c r="WR10" s="9"/>
+      <c r="WS10" s="9"/>
+      <c r="WT10" s="9"/>
+      <c r="WU10" s="9"/>
+      <c r="WV10" s="9"/>
+      <c r="WW10" s="9"/>
+      <c r="WX10" s="9"/>
+      <c r="WY10" s="9"/>
+      <c r="WZ10" s="9"/>
+      <c r="XA10" s="9"/>
+      <c r="XB10" s="9"/>
+      <c r="XC10" s="9"/>
+      <c r="XD10" s="9"/>
+      <c r="XE10" s="9"/>
+      <c r="XF10" s="9"/>
+      <c r="XG10" s="9"/>
+      <c r="XH10" s="9"/>
+      <c r="XI10" s="9"/>
+      <c r="XJ10" s="9"/>
+      <c r="XK10" s="9"/>
+      <c r="XL10" s="9"/>
+      <c r="XM10" s="9"/>
+      <c r="XN10" s="9"/>
+      <c r="XO10" s="9"/>
+      <c r="XP10" s="9"/>
+      <c r="XQ10" s="9"/>
+      <c r="XR10" s="9"/>
+      <c r="XS10" s="9"/>
+      <c r="XT10" s="9"/>
+      <c r="XU10" s="9"/>
+      <c r="XV10" s="9"/>
+      <c r="XW10" s="9"/>
+      <c r="XX10" s="9"/>
+      <c r="XY10" s="9"/>
+      <c r="XZ10" s="9"/>
+      <c r="YA10" s="9"/>
+      <c r="YB10" s="9"/>
+      <c r="YC10" s="9"/>
+      <c r="YD10" s="9"/>
+      <c r="YE10" s="9"/>
+      <c r="YF10" s="9"/>
+      <c r="YG10" s="9"/>
+      <c r="YH10" s="9"/>
+      <c r="YI10" s="9"/>
+      <c r="YJ10" s="9"/>
+      <c r="YK10" s="9"/>
+      <c r="YL10" s="9"/>
+      <c r="YM10" s="9"/>
+      <c r="YN10" s="9"/>
+      <c r="YO10" s="9"/>
+      <c r="YP10" s="9"/>
+      <c r="YQ10" s="9"/>
+      <c r="YR10" s="9"/>
+      <c r="YS10" s="9"/>
+      <c r="YT10" s="9"/>
+      <c r="YU10" s="9"/>
+      <c r="YV10" s="9"/>
+      <c r="YW10" s="9"/>
+      <c r="YX10" s="9"/>
+      <c r="YY10" s="9"/>
+      <c r="YZ10" s="9"/>
+      <c r="ZA10" s="9"/>
+      <c r="ZB10" s="9"/>
+      <c r="ZC10" s="9"/>
+      <c r="ZD10" s="9"/>
+      <c r="ZE10" s="9"/>
+      <c r="ZF10" s="9"/>
+      <c r="ZG10" s="9"/>
+      <c r="ZH10" s="9"/>
+      <c r="ZI10" s="9"/>
+      <c r="ZJ10" s="9"/>
+      <c r="ZK10" s="9"/>
+      <c r="ZL10" s="9"/>
+      <c r="ZM10" s="9"/>
+      <c r="ZN10" s="9"/>
+      <c r="ZO10" s="9"/>
+      <c r="ZP10" s="9"/>
+      <c r="ZQ10" s="9"/>
+      <c r="ZR10" s="9"/>
+      <c r="ZS10" s="9"/>
+      <c r="ZT10" s="9"/>
+      <c r="ZU10" s="9"/>
+      <c r="ZV10" s="9"/>
+      <c r="ZW10" s="9"/>
+      <c r="ZX10" s="9"/>
+      <c r="ZY10" s="9"/>
+      <c r="ZZ10" s="9"/>
+      <c r="AAA10" s="9"/>
+      <c r="AAB10" s="9"/>
+      <c r="AAC10" s="9"/>
+      <c r="AAD10" s="9"/>
+      <c r="AAE10" s="9"/>
+      <c r="AAF10" s="9"/>
+      <c r="AAG10" s="9"/>
+      <c r="AAH10" s="9"/>
+      <c r="AAI10" s="9"/>
+      <c r="AAJ10" s="9"/>
+      <c r="AAK10" s="9"/>
+      <c r="AAL10" s="9"/>
+      <c r="AAM10" s="9"/>
+      <c r="AAN10" s="9"/>
+      <c r="AAO10" s="9"/>
+      <c r="AAP10" s="9"/>
+      <c r="AAQ10" s="9"/>
+      <c r="AAR10" s="9"/>
+      <c r="AAS10" s="9"/>
+      <c r="AAT10" s="9"/>
+      <c r="AAU10" s="9"/>
+      <c r="AAV10" s="9"/>
+      <c r="AAW10" s="9"/>
+      <c r="AAX10" s="9"/>
+      <c r="AAY10" s="9"/>
+      <c r="AAZ10" s="9"/>
+      <c r="ABA10" s="9"/>
+      <c r="ABB10" s="9"/>
+      <c r="ABC10" s="9"/>
+      <c r="ABD10" s="9"/>
+      <c r="ABE10" s="9"/>
+      <c r="ABF10" s="9"/>
+      <c r="ABG10" s="9"/>
+      <c r="ABH10" s="9"/>
+      <c r="ABI10" s="9"/>
+      <c r="ABJ10" s="9"/>
+      <c r="ABK10" s="9"/>
+      <c r="ABL10" s="9"/>
+      <c r="ABM10" s="9"/>
+      <c r="ABN10" s="9"/>
+      <c r="ABO10" s="9"/>
+      <c r="ABP10" s="9"/>
+      <c r="ABQ10" s="9"/>
+      <c r="ABR10" s="9"/>
+      <c r="ABS10" s="9"/>
+      <c r="ABT10" s="9"/>
+      <c r="ABU10" s="9"/>
+      <c r="ABV10" s="9"/>
+      <c r="ABW10" s="9"/>
+      <c r="ABX10" s="9"/>
+      <c r="ABY10" s="9"/>
+      <c r="ABZ10" s="9"/>
+      <c r="ACA10" s="9"/>
+      <c r="ACB10" s="9"/>
+      <c r="ACC10" s="9"/>
+      <c r="ACD10" s="9"/>
+      <c r="ACE10" s="9"/>
+      <c r="ACF10" s="9"/>
+      <c r="ACG10" s="9"/>
+      <c r="ACH10" s="9"/>
+      <c r="ACI10" s="9"/>
+      <c r="ACJ10" s="9"/>
+      <c r="ACK10" s="9"/>
+      <c r="ACL10" s="9"/>
+      <c r="ACM10" s="9"/>
+      <c r="ACN10" s="9"/>
+      <c r="ACO10" s="9"/>
+      <c r="ACP10" s="9"/>
+      <c r="ACQ10" s="9"/>
+      <c r="ACR10" s="9"/>
+      <c r="ACS10" s="9"/>
+      <c r="ACT10" s="9"/>
+      <c r="ACU10" s="9"/>
+      <c r="ACV10" s="9"/>
+      <c r="ACW10" s="9"/>
+      <c r="ACX10" s="9"/>
+      <c r="ACY10" s="9"/>
+      <c r="ACZ10" s="9"/>
+      <c r="ADA10" s="9"/>
+      <c r="ADB10" s="9"/>
+      <c r="ADC10" s="9"/>
+      <c r="ADD10" s="9"/>
+      <c r="ADE10" s="9"/>
+      <c r="ADF10" s="9"/>
+      <c r="ADG10" s="9"/>
+      <c r="ADH10" s="9"/>
+      <c r="ADI10" s="9"/>
+      <c r="ADJ10" s="9"/>
+      <c r="ADK10" s="9"/>
+      <c r="ADL10" s="9"/>
+      <c r="ADM10" s="9"/>
+      <c r="ADN10" s="9"/>
+      <c r="ADO10" s="9"/>
+      <c r="ADP10" s="9"/>
+      <c r="ADQ10" s="9"/>
+      <c r="ADR10" s="9"/>
+      <c r="ADS10" s="9"/>
+      <c r="ADT10" s="9"/>
+      <c r="ADU10" s="9"/>
+      <c r="ADV10" s="9"/>
+      <c r="ADW10" s="9"/>
+      <c r="ADX10" s="9"/>
+      <c r="ADY10" s="9"/>
+      <c r="ADZ10" s="9"/>
+      <c r="AEA10" s="9"/>
+      <c r="AEB10" s="9"/>
+      <c r="AEC10" s="9"/>
+      <c r="AED10" s="9"/>
+      <c r="AEE10" s="9"/>
+      <c r="AEF10" s="9"/>
+      <c r="AEG10" s="9"/>
+      <c r="AEH10" s="9"/>
+      <c r="AEI10" s="9"/>
+      <c r="AEJ10" s="9"/>
+      <c r="AEK10" s="9"/>
+      <c r="AEL10" s="9"/>
+      <c r="AEM10" s="9"/>
+      <c r="AEN10" s="9"/>
+      <c r="AEO10" s="9"/>
+      <c r="AEP10" s="9"/>
+      <c r="AEQ10" s="9"/>
+      <c r="AER10" s="9"/>
+      <c r="AES10" s="9"/>
+      <c r="AET10" s="9"/>
+      <c r="AEU10" s="9"/>
+      <c r="AEV10" s="9"/>
+      <c r="AEW10" s="9"/>
+      <c r="AEX10" s="9"/>
+      <c r="AEY10" s="9"/>
+      <c r="AEZ10" s="9"/>
+      <c r="AFA10" s="9"/>
+      <c r="AFB10" s="9"/>
+      <c r="AFC10" s="9"/>
+      <c r="AFD10" s="9"/>
+      <c r="AFE10" s="9"/>
+      <c r="AFF10" s="9"/>
+      <c r="AFG10" s="9"/>
+      <c r="AFH10" s="9"/>
+      <c r="AFI10" s="9"/>
+      <c r="AFJ10" s="9"/>
+      <c r="AFK10" s="9"/>
+      <c r="AFL10" s="9"/>
+      <c r="AFM10" s="9"/>
+      <c r="AFN10" s="9"/>
+      <c r="AFO10" s="9"/>
+      <c r="AFP10" s="9"/>
+      <c r="AFQ10" s="9"/>
+      <c r="AFR10" s="9"/>
+      <c r="AFS10" s="9"/>
+      <c r="AFT10" s="9"/>
+      <c r="AFU10" s="9"/>
+      <c r="AFV10" s="9"/>
+      <c r="AFW10" s="9"/>
+      <c r="AFX10" s="9"/>
+      <c r="AFY10" s="9"/>
+      <c r="AFZ10" s="9"/>
+      <c r="AGA10" s="9"/>
+      <c r="AGB10" s="9"/>
+      <c r="AGC10" s="9"/>
+      <c r="AGD10" s="9"/>
+      <c r="AGE10" s="9"/>
+      <c r="AGF10" s="9"/>
+      <c r="AGG10" s="9"/>
+      <c r="AGH10" s="9"/>
+      <c r="AGI10" s="9"/>
+      <c r="AGJ10" s="9"/>
+      <c r="AGK10" s="9"/>
+      <c r="AGL10" s="9"/>
+      <c r="AGM10" s="9"/>
+      <c r="AGN10" s="9"/>
+      <c r="AGO10" s="9"/>
+      <c r="AGP10" s="9"/>
+      <c r="AGQ10" s="9"/>
+      <c r="AGR10" s="9"/>
+      <c r="AGS10" s="9"/>
+      <c r="AGT10" s="9"/>
+      <c r="AGU10" s="9"/>
+      <c r="AGV10" s="9"/>
+      <c r="AGW10" s="9"/>
+      <c r="AGX10" s="9"/>
+      <c r="AGY10" s="9"/>
+      <c r="AGZ10" s="9"/>
+      <c r="AHA10" s="9"/>
+      <c r="AHB10" s="9"/>
+      <c r="AHC10" s="9"/>
+      <c r="AHD10" s="9"/>
+      <c r="AHE10" s="9"/>
+      <c r="AHF10" s="9"/>
+      <c r="AHG10" s="9"/>
+      <c r="AHH10" s="9"/>
+      <c r="AHI10" s="9"/>
+      <c r="AHJ10" s="9"/>
+      <c r="AHK10" s="9"/>
+      <c r="AHL10" s="9"/>
+      <c r="AHM10" s="9"/>
+      <c r="AHN10" s="9"/>
+      <c r="AHO10" s="9"/>
+      <c r="AHP10" s="9"/>
+      <c r="AHQ10" s="9"/>
+      <c r="AHR10" s="9"/>
+      <c r="AHS10" s="9"/>
+      <c r="AHT10" s="9"/>
+      <c r="AHU10" s="9"/>
+      <c r="AHV10" s="9"/>
+      <c r="AHW10" s="9"/>
+      <c r="AHX10" s="9"/>
+      <c r="AHY10" s="9"/>
+    </row>
+    <row r="11" spans="1:909" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -730,8 +1634,8 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:909" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -746,8 +1650,8 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+    <row r="13" spans="1:909" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
@@ -758,8 +1662,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+    <row r="14" spans="1:909" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
@@ -770,7 +1674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:909" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
         <v>47</v>
@@ -782,8 +1686,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:909" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
@@ -875,14 +1779,14 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
design letter for faceuploading and %
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51412F28-75E3-4C35-8168-65A8443860BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE9F28-B10F-4F4C-B345-BC7D339C0C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,10 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$7:$D$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$7:$D$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>ping</t>
   </si>
@@ -91,9 +90,6 @@
   </si>
   <si>
     <t>Subscribed Topic</t>
-  </si>
-  <si>
-    <t>person delete request</t>
   </si>
   <si>
     <t xml:space="preserve">update time request </t>
@@ -212,6 +208,21 @@
   </si>
   <si>
     <t>NNDE = Nack for name data error</t>
+  </si>
+  <si>
+    <t>person delete request single person</t>
+  </si>
+  <si>
+    <t>imagelen +width+hight+person name+ person id+ total chank</t>
+  </si>
+  <si>
+    <t>sent image info</t>
+  </si>
+  <si>
+    <t>person id+chank no+ image data</t>
+  </si>
+  <si>
+    <t>sent image data chank</t>
   </si>
 </sst>
 </file>
@@ -651,16 +662,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A7:AHY27"/>
+  <dimension ref="A7:AHY29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
     <col min="3" max="3" width="64.28515625" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" customWidth="1"/>
   </cols>
@@ -676,7 +687,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -689,10 +700,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -713,13 +724,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -1645,7 +1656,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1656,43 +1667,39 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:909" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:909" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="5" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:909" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:909" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:909" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>28</v>
@@ -1700,114 +1707,138 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8" t="s">
+      <c r="C26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="D27" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>27</v>
+      <c r="B29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
via quaue rtoss sent log file
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE9F28-B10F-4F4C-B345-BC7D339C0C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC13A1-B692-4C24-A322-E62D1BFB05A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t xml:space="preserve">D=log time + person id </t>
   </si>
   <si>
-    <t>device time+D1+D2+…............Dn</t>
-  </si>
-  <si>
     <t>yyyy-mm-dd-hh-mm-ss-24H</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>sent image data chank</t>
+  </si>
+  <si>
+    <t>D1+D2+…............Dn</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <dimension ref="A7:AHY29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +700,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -724,7 +724,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>35</v>
@@ -1676,20 +1676,20 @@
     <row r="14" spans="1:909" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:909" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -1699,7 +1699,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>28</v>
@@ -1708,13 +1708,13 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1776,10 +1776,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>24</v>
@@ -1791,7 +1791,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>23</v>
@@ -1803,7 +1803,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>22</v>
@@ -1812,13 +1812,13 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
resize chank size and event feedback now in binary
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEEB7A2-26C9-4752-86E1-7F290B71C246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2015AA2F-4B35-4238-B6A1-7DA99954EFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -622,8 +622,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -973,8 +971,8 @@
   </sheetPr>
   <dimension ref="A2:AIA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,127 +993,127 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="23"/>
       <c r="C2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="25">
         <v>30</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>45575.507002314815</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="25" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="25">
         <v>11000</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="25">
         <v>100</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="25">
         <v>110</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="25">
         <v>11</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -2126,11 +2124,11 @@
         <v>38</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>

</xml_diff>

<commit_message>
enroll crc done and image sent done for binary data
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2015AA2F-4B35-4238-B6A1-7DA99954EFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DDCAF6-CA57-4F93-8586-93F23483D71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$15:$F$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$15:$F$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="145">
   <si>
     <t>ping</t>
   </si>
@@ -281,12 +281,6 @@
     <t>time&lt;space&gt;yyyy-mm-dd-hh-mm-ss</t>
   </si>
   <si>
-    <t>cmddl&lt;space&gt;person id&lt;space&gt; person name&lt;space&gt;crc&lt;space&gt;cndend</t>
-  </si>
-  <si>
-    <t>cmdenrol&lt;space&gt;person_name&lt;space&gt;crc_value&lt;space&gt;cmdend</t>
-  </si>
-  <si>
     <t>4E 44 50</t>
   </si>
   <si>
@@ -333,12 +327,6 @@
   </si>
   <si>
     <t xml:space="preserve">Discription  </t>
-  </si>
-  <si>
-    <t>74 69 6D 65 20 18 0A 0A 0C 0A 05 0C/18</t>
-  </si>
-  <si>
-    <t>time&lt;space&gt;24-10-10-12-10-05-12/24</t>
   </si>
   <si>
     <t>84 18 0A 0A 0C 0A 05 54 68 75 0C/18</t>
@@ -348,9 +336,6 @@
 T-24-10-10-12-10-05-Thu-12/24= 1 byte data type (T)+9 byte time stamp(24-10-10-12-10-05-Thu) + 1 byte time formet(12/24)</t>
   </si>
   <si>
-    <t>cmdenrol&lt;space&gt;Sozib&lt;space&gt; ì7 &lt;space&gt;cmdend</t>
-  </si>
-  <si>
     <t>4C 18 0A 0A 0C 0A 05 0C/18 00 1E</t>
   </si>
   <si>
@@ -386,12 +371,6 @@
     <t>Thu</t>
   </si>
   <si>
-    <t>63 6D 64 64 6C 20 00 1E 20 53 6F 7A 69 62 20 EC 37 20 63 6E 64 65 6E 64</t>
-  </si>
-  <si>
-    <t>63 6D 64 65 6E 72 6F 6C 20 53 6F 7A 69 62 20 00 DB 20 63 6D 64 65 6E 64</t>
-  </si>
-  <si>
     <t>delete crc</t>
   </si>
   <si>
@@ -453,13 +432,58 @@
   </si>
   <si>
     <t>Data frame  From Server</t>
+  </si>
+  <si>
+    <t>74 69 6D 65 20 18 0A 0A 0C 0A 05</t>
+  </si>
+  <si>
+    <t>time&lt;space&gt;24-10-10-12-10-05</t>
+  </si>
+  <si>
+    <t>ATU</t>
+  </si>
+  <si>
+    <t>ATFU</t>
+  </si>
+  <si>
+    <t>ack from device</t>
+  </si>
+  <si>
+    <t>41 54 55</t>
+  </si>
+  <si>
+    <t>41 54 46 55</t>
+  </si>
+  <si>
+    <t>cmdenrol&lt;space&gt;person_name&lt;space&gt;crc_value</t>
+  </si>
+  <si>
+    <t>63 6D 64 65 6E 72 6F 6C 20 53 6F 7A 69 62 20 00 DB</t>
+  </si>
+  <si>
+    <t>cmdenrol&lt;space&gt;Sozib&lt;space&gt; ì7</t>
+  </si>
+  <si>
+    <t>cmddl&lt;space&gt; person name&lt;space&gt;person id&lt;space&gt;crc</t>
+  </si>
+  <si>
+    <t>63 6D 64 64 6C 20 53 6F 7A 69 62 20 00 1E 20 00 00</t>
+  </si>
+  <si>
+    <t>giveimage</t>
+  </si>
+  <si>
+    <t>67 69 76 65 69 6D 61 67 65 20 01</t>
+  </si>
+  <si>
+    <t>giveimage&lt;space&gt;person_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +510,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -520,7 +549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -576,11 +605,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -606,7 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -631,6 +672,11 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,10 +1015,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AIA48"/>
+  <dimension ref="A2:AIA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,123 +1039,123 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="24">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="25">
+        <v>45575.507002314815</v>
+      </c>
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="C6" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="B8" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="25">
-        <v>30</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="26">
-        <v>45575.507002314815</v>
-      </c>
-      <c r="C5" s="25"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B10" s="24">
+        <v>11000</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="24">
+        <v>100</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="24">
+        <v>110</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="B13" s="24">
+        <v>11</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>128</v>
-      </c>
-      <c r="B10" s="25">
-        <v>11000</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="25">
-        <v>100</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="25">
-        <v>110</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="25">
-        <v>11</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1117,23 +1163,23 @@
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="15" t="s">
+      <c r="C15" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>97</v>
+      <c r="F15" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1145,15 +1191,15 @@
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1166,13 +1212,13 @@
         <v>6</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>26</v>
@@ -2090,14 +2136,14 @@
         <v>7</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="D18" s="11"/>
-      <c r="E18" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>102</v>
+      <c r="E18" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -2111,183 +2157,189 @@
       <c r="D19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:911" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+        <v>142</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="D21" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>83</v>
+        <v>34</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="4" t="s">
+      <c r="E25" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
     <row r="26" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>85</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="4" t="s">
+      <c r="E32" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
@@ -2298,250 +2350,288 @@
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="L34" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M34" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="N34" s="10" t="s">
-        <v>69</v>
-      </c>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>73</v>
+        <v>21</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="D38" s="4"/>
+      <c r="E38" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="14" t="s">
-        <v>88</v>
+        <v>58</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4" t="s">
+      <c r="C41" s="5"/>
+      <c r="D41" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="4" t="s">
+      <c r="E41" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="D43" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>90</v>
+        <v>115</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E45" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="14" t="s">
+      <c r="D50" s="4"/>
+      <c r="E50" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F48" s="5" t="s">
+      <c r="F50" s="4" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working with eventcmd and testing all event cmd
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C6646-6215-4476-97DF-C1EA000C2CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7949D9CA-6FF1-4BB6-AE63-E75437EBC289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$15:$F$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$15:$F$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="165">
   <si>
     <t>ping</t>
   </si>
@@ -180,18 +181,12 @@
     <t>sent image data chank</t>
   </si>
   <si>
-    <t xml:space="preserve">AED+person name+ Id </t>
-  </si>
-  <si>
     <t>sync</t>
   </si>
   <si>
     <t>sync image received from server</t>
   </si>
   <si>
-    <t>sync + person name + image width +image height+image data</t>
-  </si>
-  <si>
     <t>start sync</t>
   </si>
   <si>
@@ -334,9 +329,6 @@
   </si>
   <si>
     <t>68 74 69 6D 65 20 0C/18</t>
-  </si>
-  <si>
-    <t>T-yyyy-mm-dd-hh-mm-ss-12/24H</t>
   </si>
   <si>
     <t>L-d1&lt;space&gt;d2&lt;space&gt;d3…...</t>
@@ -359,9 +351,6 @@
 1byte data type (L)+ 6 byte time stamp (yyyy-mm-dd-hh-mm-ss)+1 byte time formet (12/24)+ 2 byte person id(30)&lt;space&gt;D2&lt;space&gt;D3</t>
   </si>
   <si>
-    <t>41 45 44 53 6F 7A 69 62 00 1E</t>
-  </si>
-  <si>
     <t xml:space="preserve">from device  ACK for enrol Done
 </t>
   </si>
@@ -474,22 +463,10 @@
     <t>63 6D 64 65 6E 72 6F 6C 20 53 6F 7A 69 62 20 00 DB</t>
   </si>
   <si>
-    <t>cmdenrol&lt;space&gt;Sozib&lt;space&gt; ì7</t>
-  </si>
-  <si>
     <t>cmddl&lt;space&gt; person name&lt;space&gt;person id&lt;space&gt;crc</t>
   </si>
   <si>
     <t>63 6D 64 64 6C 20 53 6F 7A 69 62 20 00 1E 20 00 00</t>
-  </si>
-  <si>
-    <t>giveimage</t>
-  </si>
-  <si>
-    <t>67 69 76 65 69 6D 61 67 65 20 01</t>
-  </si>
-  <si>
-    <t>giveimage&lt;space&gt;person_id</t>
   </si>
   <si>
     <t>delete Person Image</t>
@@ -527,6 +504,64 @@
   </si>
   <si>
     <t>4E 44 50 49 49</t>
+  </si>
+  <si>
+    <t>uploadimage&lt;space&gt;person_id</t>
+  </si>
+  <si>
+    <t>upload image</t>
+  </si>
+  <si>
+    <t>syncperson &lt;space&gt;person_name_crc&lt;space&gt; person_name&lt;space&gt;
+ image_height &lt;space&gt;image_width&lt;space&gt;image_data_crc&lt;space&gt;image_data</t>
+  </si>
+  <si>
+    <t>ASSPI</t>
+  </si>
+  <si>
+    <t>Nack for data error</t>
+  </si>
+  <si>
+    <t>NSDE</t>
+  </si>
+  <si>
+    <t>nack for saved data fail</t>
+  </si>
+  <si>
+    <t>NSSPI</t>
+  </si>
+  <si>
+    <t>41 53 53 50 49</t>
+  </si>
+  <si>
+    <t>4E 53 44 45</t>
+  </si>
+  <si>
+    <t>4E 53 53 50 49</t>
+  </si>
+  <si>
+    <t>41 53 44 20 53 6F 7A 69 62 20 00 1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AED&lt;space&gt;person name&lt;space&gt;Id </t>
+  </si>
+  <si>
+    <t>41 45 44 20 53 6F 7A 69 62 20 00 1E</t>
+  </si>
+  <si>
+    <t>73 79 6E 63 70 65 72 73 6F 6E 20 00db 20  53 6F 7A 69 62 20 02 03 20 0054 20 31 32 33 34 35 36 31 32 33 34 35 36</t>
+  </si>
+  <si>
+    <t>T-yyyy-mm-dd-hh-mm-ss-12/24</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>cmdenrol&lt;space&gt;Sozib&lt;space&gt; crc</t>
+  </si>
+  <si>
+    <t>75 70 6C 6F 61 64 69 6D 61 67 65 20 00 01</t>
   </si>
 </sst>
 </file>
@@ -559,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +616,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF669900"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -687,37 +740,76 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF33"/>
+      <color rgb="FF669900"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1049,17 +1141,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AIA54"/>
+  <dimension ref="A2:AIA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" customWidth="1"/>
+    <col min="3" max="3" width="72" customWidth="1"/>
     <col min="4" max="4" width="108" customWidth="1"/>
     <col min="5" max="5" width="86.140625" customWidth="1"/>
     <col min="6" max="6" width="88.42578125" customWidth="1"/>
@@ -1075,38 +1167,38 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B4" s="12">
         <v>30</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" s="13">
         <v>45575.507002314815</v>
@@ -1115,13 +1207,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1131,66 +1223,66 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B10" s="12">
         <v>11000</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B11" s="12">
         <v>100</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B12" s="12">
         <v>110</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B13" s="12">
         <v>11</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1201,67 +1293,67 @@
       <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>76</v>
+      <c r="C15" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="19"/>
+        <v>90</v>
+      </c>
+      <c r="G15" s="17"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="20" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E16" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="19"/>
+      <c r="F16" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="17"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:911" s="4" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="19" t="s">
+      <c r="C17" s="38"/>
+      <c r="D17" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="5"/>
@@ -2170,562 +2262,605 @@
       <c r="AIA17" s="5"/>
     </row>
     <row r="18" spans="1:911" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="G18" s="19"/>
+      <c r="C18" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" s="17"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:911" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" s="19"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:911" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:911" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="F23" s="25"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:911" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="19"/>
-    </row>
-    <row r="24" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="19"/>
-    </row>
-    <row r="25" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="19"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="28"/>
+      <c r="D26" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="19"/>
-    </row>
-    <row r="27" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="19"/>
-    </row>
-    <row r="28" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="26"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:911" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="A31" s="44"/>
+      <c r="B31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" s="30"/>
+    </row>
+    <row r="32" spans="1:911" x14ac:dyDescent="0.25">
+      <c r="A32" s="44"/>
+      <c r="B32" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
+      <c r="B33" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="44"/>
+      <c r="B34" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C34" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="31"/>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="44"/>
+      <c r="B35" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:911" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="8" t="s">
+      <c r="C35" s="32"/>
+      <c r="D35" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
+      <c r="B36" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="32"/>
+      <c r="D36" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="8" t="s">
+      <c r="E36" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="8" t="s">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="44"/>
+      <c r="B37" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>68</v>
-      </c>
+      <c r="A38" s="14"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L38" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="N38" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="A39" s="14"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="8" t="s">
-        <v>71</v>
-      </c>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="B40" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="15"/>
       <c r="F40" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="15" t="s">
-        <v>116</v>
-      </c>
+      <c r="E41" s="15"/>
       <c r="F41" s="8" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>83</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="15"/>
       <c r="F42" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="8" t="s">
+      <c r="A43" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="D43" s="30"/>
+      <c r="E43" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="32"/>
+      <c r="B44" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="C44" s="32"/>
+      <c r="D44" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="34"/>
+      <c r="E45" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F44" s="8" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="33"/>
+      <c r="B46" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="33"/>
+      <c r="D46" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="34" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="30"/>
+      <c r="B48" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="30"/>
+      <c r="B49" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="8" t="s">
+      <c r="C49" s="32"/>
+      <c r="D49" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E49" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="30"/>
+      <c r="B50" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="31"/>
+      <c r="B51" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="32"/>
+      <c r="D51" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E48" s="15" t="s">
+      <c r="F51" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F54" s="19"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E49" s="15" t="s">
+      <c r="D55" s="19"/>
+      <c r="E55" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F49" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="15" t="s">
+      <c r="F55" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F51" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F52" s="8"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54" s="8"/>
+      <c r="F56" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
exle file modify for sync cmd
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C8768A-8BE5-463C-A6A4-31240C0E0600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79930B70-273F-4059-9D97-E41758DBA3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -544,9 +544,6 @@
     <t>41 45 44 20 53 6F 7A 69 62 20 00 1E</t>
   </si>
   <si>
-    <t>73 79 6E 63 70 65 72 73 6F 6E 20 00db 20  53 6F 7A 69 62 20 02 03 20 0054 20 31 32 33 34 35 36 31 32 33 34 35 36</t>
-  </si>
-  <si>
     <t>T-yyyy-mm-dd-hh-mm-ss-12/24</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>63 6D 64 73 79 6E 63</t>
+  </si>
+  <si>
+    <t>73 79 6E 63 70 65 72 73 6F 6E 20 00db 20  53 6F 7A 69 62 20 00 01 20 02 03 20 0054 20 31 32 33 34 35 36 31 32 33 34 35 36</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1148,8 @@
   </sheetPr>
   <dimension ref="A2:AIA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>91</v>
@@ -2281,7 +2281,7 @@
         <v>131</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G18" s="17"/>
       <c r="M18" s="1"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="17"/>
@@ -2459,11 +2459,11 @@
         <v>40</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="43" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="F30" s="30"/>
     </row>
@@ -2518,10 +2518,10 @@
         <v>45</v>
       </c>
       <c r="D34" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="31" t="s">
         <v>165</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>166</v>
       </c>
       <c r="F34" s="30"/>
     </row>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
blufi host name ok
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79930B70-273F-4059-9D97-E41758DBA3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C9112C-D9B4-4A03-A85B-2C547874219D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -1148,8 +1148,8 @@
   </sheetPr>
   <dimension ref="A2:AIA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="D30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
display image showing problem by variable type now fixed
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C9112C-D9B4-4A03-A85B-2C547874219D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86342357-6BC3-412E-A7E1-5A3A2286E353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -390,9 +390,6 @@
     <t>53 6F 7A 69 62</t>
   </si>
   <si>
-    <t>0x001E</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -465,16 +462,10 @@
     <t>cmddl&lt;space&gt; person name&lt;space&gt;person id&lt;space&gt;crc</t>
   </si>
   <si>
-    <t>63 6D 64 64 6C 20 53 6F 7A 69 62 20 00 1E 20 00 00</t>
-  </si>
-  <si>
     <t>delete Person Image</t>
   </si>
   <si>
     <t>imagedl&lt;space&gt;Person_id</t>
-  </si>
-  <si>
-    <t>69 6D 61 67 65 64 6C 20 00 1E</t>
   </si>
   <si>
     <t>ack for delete person image</t>
@@ -567,6 +558,15 @@
   </si>
   <si>
     <t>73 79 6E 63 70 65 72 73 6F 6E 20 00db 20  53 6F 7A 69 62 20 00 01 20 02 03 20 0054 20 31 32 33 34 35 36 31 32 33 34 35 36</t>
+  </si>
+  <si>
+    <t>63 6D 64 64 6C 20 53 6F 7A 69 62 20 00 01 20 0420</t>
+  </si>
+  <si>
+    <t>69 6D 61 67 65 64 6C 20 00 01</t>
+  </si>
+  <si>
+    <t>0x0001</t>
   </si>
 </sst>
 </file>
@@ -1148,17 +1148,17 @@
   </sheetPr>
   <dimension ref="A2:AIA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="72" customWidth="1"/>
-    <col min="4" max="4" width="108" customWidth="1"/>
-    <col min="5" max="5" width="86.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" customWidth="1"/>
+    <col min="5" max="5" width="59.28515625" customWidth="1"/>
     <col min="6" max="6" width="88.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
@@ -1195,10 +1195,10 @@
         <v>99</v>
       </c>
       <c r="B4" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>102</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1231,10 +1231,10 @@
         <v>103</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1248,46 +1248,46 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="12">
         <v>11000</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" s="12">
         <v>100</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="12">
         <v>110</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="12">
         <v>11</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1305,10 +1305,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>74</v>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>91</v>
@@ -2274,14 +2274,14 @@
         <v>7</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G18" s="17"/>
       <c r="M18" s="1"/>
@@ -2294,10 +2294,10 @@
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>95</v>
@@ -2307,14 +2307,14 @@
     <row r="20" spans="1:911" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="17"/>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
@@ -2335,14 +2335,14 @@
     <row r="22" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="25" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="17"/>
@@ -2350,14 +2350,14 @@
     <row r="23" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="17"/>
@@ -2365,14 +2365,14 @@
     <row r="24" spans="1:911" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="17"/>
@@ -2384,10 +2384,10 @@
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="17"/>
@@ -2459,11 +2459,11 @@
         <v>40</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F30" s="30"/>
     </row>
@@ -2474,38 +2474,38 @@
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:911" x14ac:dyDescent="0.25">
       <c r="A32" s="44"/>
       <c r="B32" s="30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="45" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
       <c r="B33" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" s="31" t="s">
         <v>152</v>
-      </c>
-      <c r="E33" s="31" t="s">
-        <v>155</v>
       </c>
       <c r="F33" s="30"/>
     </row>
@@ -2518,10 +2518,10 @@
         <v>45</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F34" s="30"/>
     </row>
@@ -2535,7 +2535,7 @@
         <v>44</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>50</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="30" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>57</v>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F43" s="30" t="s">
         <v>21</v>
@@ -2739,13 +2739,13 @@
         <v>36</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="F48" s="30" t="s">
         <v>19</v>
@@ -2819,23 +2819,23 @@
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F53" s="19" t="s">
         <v>123</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F54" s="19"/>
     </row>
@@ -2858,14 +2858,14 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F56" s="19"/>
     </row>

</xml_diff>

<commit_message>
rtc sync with time library and time ping time update from wss ok
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB9453-B613-41A4-8F4C-088F681F1B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276DA15-FC5E-4F24-B0F9-BBFC63011706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$15:$F$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$16:$F$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="161">
   <si>
     <t>ping</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Example in binary</t>
   </si>
   <si>
-    <t>time&lt;space&gt;yyyy-mm-dd-hh-mm-ss</t>
-  </si>
-  <si>
     <t>4E 44 50</t>
   </si>
   <si>
@@ -279,13 +276,6 @@
   </si>
   <si>
     <t xml:space="preserve">Discription  </t>
-  </si>
-  <si>
-    <t>84 18 0A 0A 0C 0A 05 54 68 75 0C/18</t>
-  </si>
-  <si>
-    <t>total data len is 11.
-T-24-10-10-12-10-05-Thu-12/24= 1 byte data type (T)+9 byte time stamp(24-10-10-12-10-05-Thu) + 1 byte time formet(12/24)</t>
   </si>
   <si>
     <t>4C 18 0A 0A 0C 0A 05 0C/18 00 1E</t>
@@ -377,12 +367,6 @@
     <t>Data frame  From Server</t>
   </si>
   <si>
-    <t>74 69 6D 65 20 18 0A 0A 0C 0A 05</t>
-  </si>
-  <si>
-    <t>time&lt;space&gt;24-10-10-12-10-05</t>
-  </si>
-  <si>
     <t>ATU</t>
   </si>
   <si>
@@ -474,9 +458,6 @@
     <t>41 45 44 20 53 6F 7A 69 62 20 00 1E</t>
   </si>
   <si>
-    <t>T-yyyy-mm-dd-hh-mm-ss-12/24</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -521,6 +502,31 @@
   </si>
   <si>
     <t>00 1E  20 01 20 00 25 20 [RGB565]</t>
+  </si>
+  <si>
+    <t>time&lt;space&gt;yyyy-mm-dd-ww-hh-mm-ss</t>
+  </si>
+  <si>
+    <t>T-yyyy-mm-dd-ww-hh-mm-ss-12/24</t>
+  </si>
+  <si>
+    <t>84 18 0A 0A 07 0C 0A 05 0C/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total data len is 9
+T-24-10-10-07-12-10-05-12/24= 1 byte data type (T)+7 byte time stamp(24-10-10-07-12-10-05) + 1 byte time formet(12/24) </t>
+  </si>
+  <si>
+    <t>weekday index no</t>
+  </si>
+  <si>
+    <t>    "Sun" "Mon" "Tue" "Wed" "Thu" "Fri" "Sat"</t>
+  </si>
+  <si>
+    <t>74 69 6D 65 20 18 0A 1C 01 10 20 05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time&lt;space&gt;24-10-28-1-16-32-05 </t>
   </si>
 </sst>
 </file>
@@ -642,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -758,6 +764,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1103,10 +1112,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:N60"/>
+  <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,38 +1138,38 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B5" s="8">
         <v>45575.507002314815</v>
@@ -1169,13 +1178,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1185,752 +1194,762 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B10" s="7">
         <v>11000</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B11" s="7">
         <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B12" s="7">
         <v>110</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B13" s="7">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="53"/>
+    </row>
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B16" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="42" t="s">
+      <c r="C16" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>145</v>
+      <c r="F16" s="42" t="s">
+        <v>78</v>
       </c>
       <c r="G16" s="11"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+    <row r="17" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>149</v>
+      </c>
       <c r="B17" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>141</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>84</v>
+        <v>114</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="15"/>
+        <v>7</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>136</v>
+      </c>
       <c r="E18" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="18"/>
+        <v>137</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="15" t="s">
-        <v>36</v>
-      </c>
       <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>158</v>
-      </c>
+      <c r="D20" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>151</v>
+      </c>
       <c r="E21" s="15" t="s">
         <v>152</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>124</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
+      <c r="B24" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="15"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
-      <c r="B25" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>22</v>
-      </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
       <c r="B26" s="15" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="15" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
+      <c r="B28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="E28" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="B29" s="13" t="s">
+    <row r="29" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="F29" s="13" t="s">
+      <c r="C30" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>17</v>
-      </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="49"/>
+      <c r="B32" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E32" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="49"/>
+      <c r="B33" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="14" t="s">
+      <c r="F33" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B34" s="23" t="s">
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
+      <c r="C35" s="20"/>
+      <c r="D35" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B37" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="F36" s="29"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="31" t="s">
-        <v>137</v>
+      <c r="C37" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="30" t="s">
+        <v>144</v>
       </c>
       <c r="F37" s="29"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="29" t="s">
-        <v>133</v>
+        <v>41</v>
       </c>
       <c r="C38" s="29"/>
-      <c r="D38" s="43" t="s">
-        <v>134</v>
+      <c r="D38" s="29" t="s">
+        <v>127</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="29" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C39" s="29"/>
       <c r="D39" s="43" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>148</v>
+        <v>130</v>
+      </c>
+      <c r="C40" s="29"/>
+      <c r="D40" s="43" t="s">
+        <v>131</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="29"/>
+        <v>39</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>43</v>
+      </c>
       <c r="D41" s="29" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>47</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="50"/>
       <c r="B42" s="29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
       <c r="B43" s="29" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C43" s="29"/>
       <c r="D43" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="50"/>
+      <c r="B44" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="F43" s="29" t="s">
+      <c r="E44" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B46" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="E45" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="F45" s="35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="51" t="s">
+      <c r="C46" s="33"/>
+      <c r="D46" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="44"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="40"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B48" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="36"/>
-      <c r="E47" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="F47" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="51"/>
-      <c r="B48" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36" t="s">
-        <v>113</v>
-      </c>
+      <c r="C48" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="36"/>
       <c r="E48" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="F48" s="36"/>
+        <v>159</v>
+      </c>
+      <c r="F48" s="36" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="51"/>
       <c r="B49" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="36"/>
+        <v>110</v>
+      </c>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36" t="s">
+        <v>108</v>
+      </c>
       <c r="E49" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="F49" s="36" t="s">
-        <v>20</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="51"/>
       <c r="B50" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="38" t="s">
-        <v>114</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C50" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="36"/>
       <c r="E50" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="F50" s="36"/>
-    </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="45"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="51"/>
+      <c r="B51" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="36"/>
+      <c r="D51" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="36"/>
+    </row>
+    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="45"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" s="19" t="s">
+      <c r="D53" s="19"/>
+      <c r="E53" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F53" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="52"/>
-      <c r="B53" s="19" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="52"/>
+      <c r="B54" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19" t="s">
+      <c r="C54" s="19"/>
+      <c r="D54" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E54" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="45"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="F56" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="48"/>
+      <c r="B57" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="48"/>
-      <c r="B56" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-    </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="46"/>
-      <c r="B59" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="10"/>
       <c r="F59" s="5" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="46"/>
       <c r="B60" s="5" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="10"/>
       <c r="F60" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="46"/>
+      <c r="B61" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="5" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A16:A27"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A52:A53"/>
+  <mergeCells count="8">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A17:A28"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A37:A44"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A53:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
time formet save in NVS
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9276DA15-FC5E-4F24-B0F9-BBFC63011706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4593D7E-B25C-4A02-87BF-A423B2133D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -745,6 +745,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,9 +767,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1114,8 +1114,8 @@
   </sheetPr>
   <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,10 +1260,10 @@
       <c r="A14" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="53"/>
+      <c r="C14" s="46"/>
     </row>
     <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
@@ -1289,7 +1289,7 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="48" t="s">
         <v>149</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -1310,7 +1310,7 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="15" t="s">
         <v>7</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="15" t="s">
         <v>126</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="16" t="s">
         <v>35</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="15" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1370,7 @@
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="15" t="s">
         <v>116</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="15" t="s">
         <v>118</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="15" t="s">
         <v>122</v>
       </c>
@@ -1415,11 +1415,11 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="15" t="s">
         <v>8</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="15" t="s">
         <v>30</v>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="15" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1479,7 @@
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="50" t="s">
         <v>148</v>
       </c>
       <c r="B30" s="13" t="s">
@@ -1500,7 +1500,7 @@
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="13" t="s">
         <v>10</v>
       </c>
@@ -1517,7 +1517,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="13" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1534,7 @@
       <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="14" t="s">
         <v>25</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="27" t="s">
@@ -1603,7 +1603,7 @@
       <c r="F37" s="29"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
+      <c r="A38" s="51"/>
       <c r="B38" s="29" t="s">
         <v>41</v>
       </c>
@@ -1617,7 +1617,7 @@
       <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="29" t="s">
         <v>128</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="29" t="s">
         <v>130</v>
       </c>
@@ -1645,7 +1645,7 @@
       <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="29" t="s">
         <v>39</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="29" t="s">
         <v>40</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="29" t="s">
         <v>44</v>
       </c>
@@ -1693,7 +1693,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="29" t="s">
         <v>60</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="F47" s="40"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="51" t="s">
+      <c r="A48" s="52" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="36" t="s">
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="51"/>
+      <c r="A49" s="52"/>
       <c r="B49" s="36" t="s">
         <v>110</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="F49" s="36"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="51"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="36" t="s">
         <v>62</v>
       </c>
@@ -1791,7 +1791,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="51"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="36" t="s">
         <v>110</v>
       </c>
@@ -1813,7 +1813,7 @@
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="53" t="s">
         <v>138</v>
       </c>
       <c r="B53" s="19" t="s">
@@ -1831,7 +1831,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="19" t="s">
         <v>51</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="48" t="s">
+      <c r="A56" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B56" s="21" t="s">
@@ -1873,7 +1873,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="48"/>
+      <c r="A57" s="49"/>
       <c r="B57" s="21" t="s">
         <v>51</v>
       </c>
@@ -1897,7 +1897,7 @@
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="46" t="s">
+      <c r="A59" s="47" t="s">
         <v>1</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -1913,7 +1913,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="46"/>
+      <c r="A60" s="47"/>
       <c r="B60" s="5" t="s">
         <v>56</v>
       </c>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="46"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
blufi disable in sleep
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4593D7E-B25C-4A02-87BF-A423B2133D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA19A77-088B-4679-80CA-1795E8B39FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -1114,8 +1114,8 @@
   </sheetPr>
   <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bug at checking valid recognize this bug created problem with enrolment process
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA19A77-088B-4679-80CA-1795E8B39FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E95670C-6260-4087-A21C-07610BB7565D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$16:$F$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$17:$F$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="162">
   <si>
     <t>ping</t>
   </si>
@@ -520,20 +520,250 @@
     <t>weekday index no</t>
   </si>
   <si>
-    <t>    "Sun" "Mon" "Tue" "Wed" "Thu" "Fri" "Sat"</t>
-  </si>
-  <si>
     <t>74 69 6D 65 20 18 0A 1C 01 10 20 05</t>
   </si>
   <si>
     <t xml:space="preserve">time&lt;space&gt;24-10-28-1-16-32-05 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    0   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Sun" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Mon"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Tue"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Wed"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Thu"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Fri"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Sat"</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,6 +787,84 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF66FF33"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF66FF33"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -621,7 +929,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -644,11 +952,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -745,9 +1105,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,6 +1125,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1112,17 +1484,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:N61"/>
+  <dimension ref="A2:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
     <col min="4" max="4" width="59.42578125" customWidth="1"/>
     <col min="5" max="5" width="59.28515625" customWidth="1"/>
     <col min="6" max="6" width="88.42578125" customWidth="1"/>
@@ -1136,7 +1508,7 @@
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -1145,7 +1517,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>84</v>
       </c>
@@ -1156,7 +1528,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>85</v>
       </c>
@@ -1167,7 +1539,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>86</v>
       </c>
@@ -1176,7 +1548,7 @@
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>87</v>
       </c>
@@ -1187,12 +1559,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -1203,7 +1575,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>90</v>
       </c>
@@ -1212,7 +1584,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>99</v>
       </c>
@@ -1223,7 +1595,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>100</v>
       </c>
@@ -1234,7 +1606,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>101</v>
       </c>
@@ -1245,7 +1617,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>102</v>
       </c>
@@ -1256,700 +1628,709 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" s="46"/>
-    </row>
-    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="42" t="s">
+      <c r="B14" s="53" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="54"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
+      <c r="B15" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15" s="55"/>
+    </row>
+    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B17" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C17" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D17" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E17" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F17" s="42" t="s">
         <v>78</v>
-      </c>
-      <c r="G16" s="11"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>139</v>
       </c>
       <c r="G17" s="11"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
+    <row r="18" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>149</v>
+      </c>
       <c r="B18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F19" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="15" t="s">
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C20" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16" t="s">
+      <c r="D20" s="15"/>
+      <c r="E20" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="16" t="s">
+      <c r="F20" s="18"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
+      <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="18" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>152</v>
-      </c>
+      <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
+    <row r="22" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>151</v>
+      </c>
       <c r="E22" s="15" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
-        <v>119</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="15"/>
       <c r="E23" s="15" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="15"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="15" t="s">
+    <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="47"/>
+      <c r="B27" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="15" t="s">
-        <v>30</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="47"/>
+      <c r="B29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E29" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F29" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="25"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E31" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="13" t="s">
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="49"/>
+      <c r="B32" s="13" t="s">
         <v>10</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="13" t="s">
-        <v>11</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="49"/>
+      <c r="B33" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E33" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="14" t="s">
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="49"/>
+      <c r="B34" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B36" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="23" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E36" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F36" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="51" t="s">
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B38" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C38" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30" t="s">
+      <c r="D38" s="29"/>
+      <c r="E38" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="F37" s="29"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
-      <c r="B38" s="29" t="s">
+      <c r="F38" s="29"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="50"/>
+      <c r="B39" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29" t="s">
+      <c r="C39" s="29"/>
+      <c r="D39" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E39" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="F38" s="29"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
-      <c r="B39" s="29" t="s">
+      <c r="F39" s="29"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="50"/>
+      <c r="B40" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
-      <c r="B40" s="29" t="s">
-        <v>130</v>
       </c>
       <c r="C40" s="29"/>
       <c r="D40" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="29"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="50"/>
+      <c r="B41" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E41" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
-      <c r="B41" s="29" t="s">
+      <c r="F41" s="29"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="50"/>
+      <c r="B42" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C42" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D42" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E42" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="29"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="29" t="s">
+      <c r="F42" s="29"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="50"/>
+      <c r="B43" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="29" t="s">
-        <v>44</v>
       </c>
       <c r="C43" s="29"/>
       <c r="D43" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="29" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="50"/>
+      <c r="B45" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E45" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F45" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="B47" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="33"/>
-      <c r="D46" s="34" t="s">
+      <c r="C47" s="33"/>
+      <c r="D47" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="E46" s="34" t="s">
+      <c r="E47" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="F47" s="35" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="40"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="52" t="s">
+    <row r="48" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="44"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="40"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B49" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C49" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="D48" s="36"/>
-      <c r="E48" s="37" t="s">
+      <c r="D49" s="36"/>
+      <c r="E49" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="F49" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F48" s="36" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
-      <c r="B49" s="36" t="s">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="51"/>
+      <c r="B50" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36" t="s">
+      <c r="C50" s="36"/>
+      <c r="D50" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="E50" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F49" s="36"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
-      <c r="B50" s="36" t="s">
+      <c r="F50" s="36"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="51"/>
+      <c r="B51" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C51" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37" t="s">
+      <c r="D51" s="36"/>
+      <c r="E51" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="F50" s="36" t="s">
+      <c r="F51" s="36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="52"/>
-      <c r="B51" s="36" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="51"/>
+      <c r="B52" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="38" t="s">
+      <c r="C52" s="36"/>
+      <c r="D52" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="37" t="s">
+      <c r="E52" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F51" s="36"/>
-    </row>
-    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="53" t="s">
+      <c r="F52" s="36"/>
+    </row>
+    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="45"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B54" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C54" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="20" t="s">
+      <c r="D54" s="19"/>
+      <c r="E54" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="F54" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="53"/>
-      <c r="B54" s="19" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="52"/>
+      <c r="B55" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="20" t="s">
+      <c r="E55" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F55" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="45"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="5"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="s">
+    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="45"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B57" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C57" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="22" t="s">
+      <c r="D57" s="21"/>
+      <c r="E57" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F57" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="49"/>
-      <c r="B57" s="21" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="48"/>
+      <c r="B58" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21" t="s">
+      <c r="C58" s="21"/>
+      <c r="D58" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="E58" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F58" s="21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
-      <c r="B60" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="10"/>
       <c r="F60" s="5" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
+      <c r="A61" s="46"/>
       <c r="B61" s="5" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="10"/>
       <c r="F61" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="46"/>
+      <c r="B62" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="5" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A17:A28"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A37:A44"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A53:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rtc time handle for invalid rtc
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E95670C-6260-4087-A21C-07610BB7565D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE54FFB-63F4-422B-8539-3C141119EE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -1105,6 +1105,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1126,20 +1129,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1487,7 +1487,7 @@
   <dimension ref="A2:N62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,20 +1629,20 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="54"/>
+      <c r="C14" s="57"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="55" t="s">
+      <c r="A15" s="55"/>
+      <c r="B15" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="C15" s="55"/>
+      <c r="C15" s="46"/>
     </row>
     <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="42" t="s">
@@ -1668,7 +1668,7 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="48" t="s">
         <v>149</v>
       </c>
       <c r="B18" s="15" t="s">
@@ -1689,7 +1689,7 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="15" t="s">
         <v>126</v>
       </c>
@@ -1721,7 +1721,7 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="15" t="s">
         <v>36</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="15" t="s">
         <v>116</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="15" t="s">
         <v>118</v>
       </c>
@@ -1779,7 +1779,7 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="15" t="s">
         <v>122</v>
       </c>
@@ -1794,11 +1794,11 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="15" t="s">
         <v>8</v>
       </c>
@@ -1815,7 +1815,7 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="15" t="s">
         <v>30</v>
       </c>
@@ -1832,7 +1832,7 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="15" t="s">
         <v>9</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="50" t="s">
         <v>148</v>
       </c>
       <c r="B31" s="13" t="s">
@@ -1879,7 +1879,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="13" t="s">
         <v>10</v>
       </c>
@@ -1896,7 +1896,7 @@
       <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="13" t="s">
         <v>11</v>
       </c>
@@ -1913,7 +1913,7 @@
       <c r="G33" s="11"/>
     </row>
     <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="14" t="s">
         <v>25</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
@@ -1982,7 +1982,7 @@
       <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="29" t="s">
         <v>41</v>
       </c>
@@ -1996,7 +1996,7 @@
       <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="29" t="s">
         <v>128</v>
       </c>
@@ -2010,7 +2010,7 @@
       <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="29" t="s">
         <v>130</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="29" t="s">
         <v>39</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="29" t="s">
         <v>40</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="29" t="s">
         <v>44</v>
       </c>
@@ -2072,7 +2072,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="29" t="s">
         <v>60</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="F48" s="40"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="52" t="s">
         <v>2</v>
       </c>
       <c r="B49" s="36" t="s">
@@ -2140,7 +2140,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="51"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="36" t="s">
         <v>110</v>
       </c>
@@ -2154,7 +2154,7 @@
       <c r="F50" s="36"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="51"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="36" t="s">
         <v>62</v>
       </c>
@@ -2170,7 +2170,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="51"/>
+      <c r="A52" s="52"/>
       <c r="B52" s="36" t="s">
         <v>110</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="52" t="s">
+      <c r="A54" s="53" t="s">
         <v>138</v>
       </c>
       <c r="B54" s="19" t="s">
@@ -2210,7 +2210,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="52"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="19" t="s">
         <v>51</v>
       </c>
@@ -2234,7 +2234,7 @@
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="48" t="s">
+      <c r="A57" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B57" s="21" t="s">
@@ -2252,7 +2252,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="48"/>
+      <c r="A58" s="49"/>
       <c r="B58" s="21" t="s">
         <v>51</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+      <c r="A60" s="47" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -2292,7 +2292,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="46"/>
+      <c r="A61" s="47"/>
       <c r="B61" s="5" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="46"/>
+      <c r="A62" s="47"/>
       <c r="B62" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
improved wss connection process
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE54FFB-63F4-422B-8539-3C141119EE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC8003-701D-444D-8F2D-1F92B5B124ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -1487,7 +1487,7 @@
   <dimension ref="A2:N62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:C14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
optimize time lib for less clock use
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC8003-701D-444D-8F2D-1F92B5B124ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A23CA-077B-4F07-8FCA-7F1C12CF2136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -1486,8 +1486,8 @@
   </sheetPr>
   <dimension ref="A2:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add battry in ping payload
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A23CA-077B-4F07-8FCA-7F1C12CF2136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62969D-C69B-4A93-A86B-DE975612291B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -507,16 +507,6 @@
     <t>time&lt;space&gt;yyyy-mm-dd-ww-hh-mm-ss</t>
   </si>
   <si>
-    <t>T-yyyy-mm-dd-ww-hh-mm-ss-12/24</t>
-  </si>
-  <si>
-    <t>84 18 0A 0A 07 0C 0A 05 0C/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total data len is 9
-T-24-10-10-07-12-10-05-12/24= 1 byte data type (T)+7 byte time stamp(24-10-10-07-12-10-05) + 1 byte time formet(12/24) </t>
-  </si>
-  <si>
     <t>weekday index no</t>
   </si>
   <si>
@@ -757,6 +747,16 @@
       </rPr>
       <t>"Sat"</t>
     </r>
+  </si>
+  <si>
+    <t>T-yyyy-mm-dd-ww-hh-mm-ss-12/24-rssi-bat value</t>
+  </si>
+  <si>
+    <t>84 18 0A 0A 07 0C 0A 05 0C/18 5A 05 DC</t>
+  </si>
+  <si>
+    <t>total data len is 12
+T-24-10-10-07-12-10-05-12/24-5A-05 DC= 1 byte data type (T)+ 8 byte time stamp(24-10-10-07-12-10-05) + 1 byte time formet(12/24)+1  byte wifi rssi + 2 byte battry voltage in mv</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1486,8 @@
   </sheetPr>
   <dimension ref="A2:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,17 +1630,17 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="56" t="s">
         <v>157</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>160</v>
       </c>
       <c r="C14" s="57"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="55"/>
       <c r="B15" s="46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C15" s="46"/>
     </row>
@@ -2099,18 +2099,18 @@
       <c r="A47" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="33" t="s">
+      <c r="B47" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="33"/>
       <c r="D47" s="34" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F47" s="35" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2133,10 +2133,10 @@
       </c>
       <c r="D49" s="36"/>
       <c r="E49" s="37" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F49" s="36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add blufi protocal cmd list for wifi settigs
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62969D-C69B-4A93-A86B-DE975612291B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03E7D6-CF72-43A8-AF7D-A6F400116251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$17:$F$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$33:$F$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="190">
   <si>
     <t>ping</t>
   </si>
@@ -319,21 +319,12 @@
     <t>0x00DB</t>
   </si>
   <si>
-    <t>in binary</t>
-  </si>
-  <si>
-    <t>53 6F 7A 69 62</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>0xec37</t>
   </si>
   <si>
-    <t>54 68 75</t>
-  </si>
-  <si>
     <t>63 6C 65 61 6E</t>
   </si>
   <si>
@@ -350,9 +341,6 @@
   </si>
   <si>
     <t>total chank</t>
-  </si>
-  <si>
-    <t>2AF8</t>
   </si>
   <si>
     <t>0x64</t>
@@ -758,12 +746,108 @@
     <t>total data len is 12
 T-24-10-10-07-12-10-05-12/24-5A-05 DC= 1 byte data type (T)+ 8 byte time stamp(24-10-10-07-12-10-05) + 1 byte time formet(12/24)+1  byte wifi rssi + 2 byte battry voltage in mv</t>
   </si>
+  <si>
+    <t>wifi configure</t>
+  </si>
+  <si>
+    <t>Request name</t>
+  </si>
+  <si>
+    <t>OPMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD </t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>08 08 +Transection No + 01 01</t>
+  </si>
+  <si>
+    <t>SSID</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>09 00 + Transection No + Data len+ SSID</t>
+  </si>
+  <si>
+    <t>0D 00 +Transection No + Data len + PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect request </t>
+  </si>
+  <si>
+    <t>0C 00 + Transection No + 00</t>
+  </si>
+  <si>
+    <t>Wifi ssid</t>
+  </si>
+  <si>
+    <t>myssid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass </t>
+  </si>
+  <si>
+    <t>mypassword</t>
+  </si>
+  <si>
+    <t>ssid len</t>
+  </si>
+  <si>
+    <t>pass len</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> binary</t>
+  </si>
+  <si>
+    <t>0x53  0x6F 0x7A  0x69 0x62</t>
+  </si>
+  <si>
+    <t>0x54 0x68 0x75</t>
+  </si>
+  <si>
+    <t>0x2AF8</t>
+  </si>
+  <si>
+    <t>0x6D 0x79 0x73 0x73 0x69 0x64</t>
+  </si>
+  <si>
+    <t>0x6D 0x79 0x70 0x61 0x73 0x73 0x77 0x6F 0x72 0x64</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x08 0x08 0x00 0x01 0x01</t>
+  </si>
+  <si>
+    <t>0x09 0x00 0x01 0x06 0x6D 0x79 0x73 0x73 0x69 0x64</t>
+  </si>
+  <si>
+    <t>0x0D 0x00 0x02 0x0A 0x6D 0x79 0x70 0x61 0x73 0x73 0x77 0x6F 0x72 0x64</t>
+  </si>
+  <si>
+    <t>0x0C 0x00 0x03 0x00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,8 +950,22 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,8 +1026,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1004,11 +1108,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1140,6 +1253,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1484,17 +1619,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:N62"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" customWidth="1"/>
     <col min="4" max="4" width="59.42578125" customWidth="1"/>
     <col min="5" max="5" width="59.28515625" customWidth="1"/>
     <col min="6" max="6" width="88.42578125" customWidth="1"/>
@@ -1508,13 +1643,22 @@
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>92</v>
+      <c r="A2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1669,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>93</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1536,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1556,7 +1700,7 @@
         <v>88</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>96</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1569,10 +1713,10 @@
         <v>89</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,751 +1730,864 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B10" s="7">
         <v>11000</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>103</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B11" s="7">
         <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="7">
         <v>110</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B13" s="7">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C14" s="57"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="55"/>
       <c r="B15" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="46"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" s="7">
+        <v>6</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" s="7">
+        <v>10</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="46"/>
-    </row>
-    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="42" t="s">
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="62" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A33" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B33" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="42" t="s">
+      <c r="C33" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F33" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="G33" s="11"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C34" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="11"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="48"/>
+      <c r="B35" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
+      <c r="B36" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="48"/>
+      <c r="B37" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="48"/>
+      <c r="B38" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="15"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="48"/>
+      <c r="B39" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16" t="s">
+      <c r="D39" s="15"/>
+      <c r="E39" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="15"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="48"/>
+      <c r="B40" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="48"/>
+      <c r="B41" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="48"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="48"/>
+      <c r="B43" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="48"/>
+      <c r="B44" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="48"/>
+      <c r="B45" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="50"/>
+      <c r="B48" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="50"/>
+      <c r="B49" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="50"/>
+      <c r="B50" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="25"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="29"/>
+      <c r="E54" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="F54" s="29"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="51"/>
+      <c r="B55" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="29"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="51"/>
+      <c r="B56" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="29"/>
+      <c r="D56" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="F56" s="29"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="51"/>
+      <c r="B57" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="29"/>
+      <c r="D57" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="29"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="51"/>
+      <c r="B58" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E58" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
-      <c r="B29" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" s="29"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
-      <c r="B39" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
-      <c r="B40" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
-      <c r="B41" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="43" t="s">
+      <c r="F58" s="29"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="51"/>
+      <c r="B59" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E59" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="29"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="F42" s="29"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="29" t="s">
+      <c r="F59" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
-      <c r="B44" s="29" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="51"/>
+      <c r="B60" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
+      <c r="C60" s="29"/>
+      <c r="D60" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E60" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F60" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
-      <c r="B45" s="29" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="51"/>
+      <c r="B61" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29" t="s">
+      <c r="C61" s="29"/>
+      <c r="D61" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E61" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="29" t="s">
+      <c r="F61" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="F47" s="35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="40"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="F49" s="36" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
-      <c r="B50" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="E50" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="36"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="52"/>
-      <c r="B51" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="F51" s="36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
-      <c r="B52" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="E52" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="F52" s="36"/>
-    </row>
-    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D54" s="19"/>
-      <c r="E54" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="53"/>
-      <c r="B55" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="49"/>
-      <c r="B58" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
-      <c r="B61" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
-      <c r="B62" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>24</v>
-      </c>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="9"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="10"/>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="33"/>
+      <c r="D63" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E63" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="44"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="40"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="36"/>
+      <c r="E65" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F65" s="36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="52"/>
+      <c r="B66" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E66" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F66" s="36"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="52"/>
+      <c r="B67" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" s="36"/>
+      <c r="E67" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F67" s="36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="52"/>
+      <c r="B68" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="36"/>
+      <c r="D68" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="36"/>
+    </row>
+    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="45"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D70" s="19"/>
+      <c r="E70" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="53"/>
+      <c r="B71" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F71" s="19" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="72" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="45"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="21"/>
+      <c r="E73" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="49"/>
+      <c r="B74" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="47"/>
+      <c r="B77" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="47"/>
+      <c r="B78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A34:A45"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A54:A61"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A70:A71"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add crc and wifi cmd list in exele file
</commit_message>
<xml_diff>
--- a/doc/cmd list.xlsx
+++ b/doc/cmd list.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62969D-C69B-4A93-A86B-DE975612291B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D532D8-06F1-432E-8BD1-5FA3484E9EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$17:$F$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$38:$F$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="196">
   <si>
     <t>ping</t>
   </si>
@@ -230,9 +230,6 @@
     <t>time formet request</t>
   </si>
   <si>
-    <t>Example in binary</t>
-  </si>
-  <si>
     <t>4E 44 50</t>
   </si>
   <si>
@@ -279,10 +276,6 @@
   </si>
   <si>
     <t>4C 18 0A 0A 0C 0A 05 0C/18 00 1E</t>
-  </si>
-  <si>
-    <t>L-yyyy-mm-dd-hh-mm-ss-12/24-30
-1byte data type (L)+ 6 byte time stamp (yyyy-mm-dd-hh-mm-ss)+1 byte time formet (12/24)+ 2 byte person id(30)&lt;space&gt;D2&lt;space&gt;D3</t>
   </si>
   <si>
     <t xml:space="preserve">from device  ACK for enrol Done
@@ -292,9 +285,6 @@
     <t>Sozib</t>
   </si>
   <si>
-    <t>Data considered</t>
-  </si>
-  <si>
     <t>person Name</t>
   </si>
   <si>
@@ -319,21 +309,12 @@
     <t>0x00DB</t>
   </si>
   <si>
-    <t>in binary</t>
-  </si>
-  <si>
-    <t>53 6F 7A 69 62</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>0xec37</t>
   </si>
   <si>
-    <t>54 68 75</t>
-  </si>
-  <si>
     <t>63 6C 65 61 6E</t>
   </si>
   <si>
@@ -350,9 +331,6 @@
   </si>
   <si>
     <t>total chank</t>
-  </si>
-  <si>
-    <t>2AF8</t>
   </si>
   <si>
     <t>0x64</t>
@@ -758,12 +736,165 @@
     <t>total data len is 12
 T-24-10-10-07-12-10-05-12/24-5A-05 DC= 1 byte data type (T)+ 8 byte time stamp(24-10-10-07-12-10-05) + 1 byte time formet(12/24)+1  byte wifi rssi + 2 byte battry voltage in mv</t>
   </si>
+  <si>
+    <t>wifi configure</t>
+  </si>
+  <si>
+    <t>Request name</t>
+  </si>
+  <si>
+    <t>OPMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD </t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>08 08 +Transection No + 01 01</t>
+  </si>
+  <si>
+    <t>SSID</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>09 00 + Transection No + Data len+ SSID</t>
+  </si>
+  <si>
+    <t>0D 00 +Transection No + Data len + PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect request </t>
+  </si>
+  <si>
+    <t>0C 00 + Transection No + 00</t>
+  </si>
+  <si>
+    <t>Wifi ssid</t>
+  </si>
+  <si>
+    <t>myssid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass </t>
+  </si>
+  <si>
+    <t>mypassword</t>
+  </si>
+  <si>
+    <t>ssid len</t>
+  </si>
+  <si>
+    <t>pass len</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>0x53  0x6F 0x7A  0x69 0x62</t>
+  </si>
+  <si>
+    <t>0x54 0x68 0x75</t>
+  </si>
+  <si>
+    <t>0x2AF8</t>
+  </si>
+  <si>
+    <t>0x6D 0x79 0x73 0x73 0x69 0x64</t>
+  </si>
+  <si>
+    <t>0x6D 0x79 0x70 0x61 0x73 0x73 0x77 0x6F 0x72 0x64</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x08 0x08 0x00 0x01 0x01</t>
+  </si>
+  <si>
+    <t>0x09 0x00 0x01 0x06 0x6D 0x79 0x73 0x73 0x69 0x64</t>
+  </si>
+  <si>
+    <t>0x0D 0x00 0x02 0x0A 0x6D 0x79 0x70 0x61 0x73 0x73 0x77 0x6F 0x72 0x64</t>
+  </si>
+  <si>
+    <t>0x0C 0x00 0x03 0x00</t>
+  </si>
+  <si>
+    <t>Example Hex Stream</t>
+  </si>
+  <si>
+    <t>Example in Hex Stream</t>
+  </si>
+  <si>
+    <t>CMD List end</t>
+  </si>
+  <si>
+    <t>CMD List Start</t>
+  </si>
+  <si>
+    <t>Exmple Data considered</t>
+  </si>
+  <si>
+    <t>CRC Function in c</t>
+  </si>
+  <si>
+    <t>// CRC-16
+uint16_t crc16(const char *buf, size_t len) {
+    uint16_t crc = 0x0000; 
+    for (size_t i = 0; i &lt; len; i++) {
+        uint8_t byte = buf[i];
+        crc = (crc &gt;&gt; 8) ^ crc16_table[(crc &amp; 0xFF) ^ byte];
+    }
+    return crc;
+}</t>
+  </si>
+  <si>
+    <t>CRC Table</t>
+  </si>
+  <si>
+    <t>const DATA_FLASH uint16_t crc16_table[256] = 
+{
+    0x0000, 0x1021, 0x2042, 0x3063, 0x4084, 0x50a5, 0x60c6, 0x70e7,
+    0x8108, 0x9129, 0xa14a, 0xb16b, 0xc18c, 0xd1ad, 0xe1ce, 0xf1ef,
+    0x1231, 0x0210, 0x3273, 0x2252, 0x52b5, 0x4294, 0x72f7, 0x62d6,
+    0x9339, 0x8318, 0xb37b, 0xa35a, 0xd3bd, 0xc39c, 0xf3ff, 0xe3de,
+    0x2462, 0x3443, 0x0420, 0x1401, 0x64e6, 0x74c7, 0x44a4, 0x5485,
+    0xa56a, 0xb54b, 0x8528, 0x9509, 0xe5ee, 0xf5cf, 0xc5ac, 0xd58d,
+    0x3653, 0x2672, 0x1611, 0x0630, 0x76d7, 0x66f6, 0x5695, 0x46b4,
+    0xb75b, 0xa77a, 0x9719, 0x8738, 0xf7df, 0xe7fe, 0xd79d, 0xc69c,
+    0x48a4, 0x58b5, 0x6886, 0x78a7, 0x0840, 0x1861, 0x2802, 0x3823,
+    0xc9cc, 0xd9ed, 0xe98e, 0xf9af, 0x8948, 0x9969, 0xa90a, 0xb92b,
+    0x5af5, 0x4ad4, 0x7ab7, 0x6a96, 0x1a71, 0x0a50, 0x3a33, 0x2a22,
+    0xdbfd, 0xcbdc, 0xfbbf, 0xeb9e, 0x9b79, 0x8b58, 0xbb3b, 0xab1a,
+    0x6ca6, 0x7c87, 0x4404, 0x5405, 0x3403, 0x2402, 0x1401, 0x0400,
+    0xd95a, 0xc95b, 0xfca1, 0xeca2, 0x8cdd, 0x9cd9, 0xbcc3, 0xacc2,
+    0x5c8f, 0x4c9e, 0x7ea7, 0x6ea6, 0x2a12, 0x3a13, 0x0a50, 0x1a51,
+    0xf8bf, 0xe8ae, 0x9c9d, 0x8cad, 0xbab5, 0xaab4, 0x6e8f, 0x7e9e,
+    0x4f4c, 0x5f5d, 0x2d23, 0x3d32, 0x1b11, 0x0b10, 0x86d3, 0x96e2,
+    0xe6df, 0xf6cf, 0x4ed
+  };</t>
+  </si>
+  <si>
+    <t>D1 = L(hex)-yyyy-mm-dd-hh-mm-ss-12/24-30
+1byte data type (L)+ 6 byte time stamp (yyyy-mm-dd-hh-mm-ss)+1 byte time formet (12/24)+ 2 byte person id(30)
+so final groupe log like D1&lt;space&gt;D2&lt;space&gt;D3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,8 +997,22 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,8 +1073,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1004,11 +1167,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1105,6 +1288,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1135,11 +1319,55 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1484,17 +1712,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:N62"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" customWidth="1"/>
     <col min="4" max="4" width="59.42578125" customWidth="1"/>
     <col min="5" max="5" width="59.28515625" customWidth="1"/>
     <col min="6" max="6" width="88.42578125" customWidth="1"/>
@@ -1508,829 +1736,1039 @@
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="E1" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="68"/>
+      <c r="F3" s="70"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="70"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B5" s="8">
         <v>45575.507002314815</v>
       </c>
       <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="68"/>
+      <c r="F5" s="70"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="E6" s="68"/>
+      <c r="F6" s="70"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="68"/>
+      <c r="F7" s="70"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E8" s="68"/>
+      <c r="F8" s="70"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E9" s="68"/>
+      <c r="F9" s="70"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B10" s="7">
         <v>11000</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="E10" s="68"/>
+      <c r="F10" s="70"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B11" s="7">
         <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="E11" s="68"/>
+      <c r="F11" s="70"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B12" s="7">
         <v>110</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E12" s="68"/>
+      <c r="F12" s="70"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B13" s="7">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="68"/>
+      <c r="F13" s="70"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="74"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="70"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="56"/>
+      <c r="B15" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="70"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E16" s="68"/>
+      <c r="F16" s="70"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="68"/>
+      <c r="F17" s="70"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="7">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="70"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="7">
+        <v>10</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="70"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="68"/>
+      <c r="F20" s="70"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="68"/>
+      <c r="F21" s="70"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="68"/>
+      <c r="F22" s="70"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="68"/>
+      <c r="F23" s="70"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="68"/>
+      <c r="F24" s="70"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="68"/>
+      <c r="F25" s="71"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+    </row>
+    <row r="30" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="72" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="72" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="72" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A38" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="G38" s="11"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="D39" s="16"/>
+      <c r="E39" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="49"/>
+      <c r="B40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="49"/>
+      <c r="B41" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="49"/>
+      <c r="B42" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="49"/>
+      <c r="B43" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F43" s="15"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="49"/>
+      <c r="B44" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="49"/>
+      <c r="B45" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="49"/>
+      <c r="B46" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="49"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="49"/>
+      <c r="B49" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="49"/>
+      <c r="B50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="25"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="51"/>
+      <c r="B53" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="51"/>
+      <c r="B54" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="51"/>
+      <c r="B55" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="25"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="29"/>
+      <c r="E59" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F59" s="29"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="52"/>
+      <c r="B60" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="F60" s="29"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="52"/>
+      <c r="B61" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="29"/>
+      <c r="D61" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F61" s="29"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="52"/>
+      <c r="B62" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="29"/>
+      <c r="D62" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="E62" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="F62" s="29"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="52"/>
+      <c r="B63" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E63" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F63" s="29"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="52"/>
+      <c r="B64" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="52"/>
+      <c r="B65" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E65" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="52"/>
+      <c r="B66" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E66" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="9"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="33"/>
+      <c r="D68" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="E68" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F68" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="C14" s="57"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="46"/>
-    </row>
-    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+    </row>
+    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="44"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="40"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D70" s="36"/>
+      <c r="E70" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F70" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
-      <c r="B29" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="14" t="s">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="53"/>
+      <c r="B71" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="36"/>
+      <c r="D71" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71" s="36"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="53"/>
+      <c r="B72" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="F38" s="29"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
-      <c r="B39" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
-      <c r="B40" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
-      <c r="B41" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="43" t="s">
+      <c r="D72" s="36"/>
+      <c r="E72" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F72" s="36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="53"/>
+      <c r="B73" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="36"/>
+      <c r="D73" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E73" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="F73" s="36"/>
+    </row>
+    <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="45"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="29"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="F42" s="29"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
-      <c r="B44" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
-      <c r="B45" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="31" t="s">
+      <c r="B75" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="54"/>
+      <c r="B76" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E76" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="F47" s="35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="40"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="F49" s="36" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
-      <c r="B50" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="E50" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="36"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="52"/>
-      <c r="B51" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="F51" s="36" t="s">
+      <c r="F76" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="45"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" s="21"/>
+      <c r="E78" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F78" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
-      <c r="B52" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="E52" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="F52" s="36"/>
-    </row>
-    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D54" s="19"/>
-      <c r="E54" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F54" s="19" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="50"/>
+      <c r="B79" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F79" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="53"/>
-      <c r="B55" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="19" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="48"/>
+      <c r="B82" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="48"/>
+      <c r="B83" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="49"/>
-      <c r="B58" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
-      <c r="B61" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
-      <c r="B62" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="5" t="s">
-        <v>19</v>
-      </c>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="65"/>
+      <c r="C87" s="65"/>
+      <c r="D87" s="65"/>
+      <c r="E87" s="65"/>
+      <c r="F87" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="E2:E25"/>
+    <mergeCell ref="F2:F25"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A38:A45"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A39:A50"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A75:A76"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>